<commit_message>
updated Test Cases Plan
</commit_message>
<xml_diff>
--- a/tests/TestCasesPlan.xlsx
+++ b/tests/TestCasesPlan.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="120">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -57,39 +57,9 @@
     <t>LoginExpo</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">Test Different combination of Username </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>Eg</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>: Empty username,Empty password, Valid Username, Invalid Username,Invalid Password,valid password</t>
-    </r>
-  </si>
-  <si>
     <t>ExpoSKUAddNew</t>
   </si>
   <si>
-    <t>Test SKU management in Expoloader.  AddNew</t>
-  </si>
-  <si>
     <t>Amna</t>
   </si>
   <si>
@@ -108,30 +78,18 @@
     <t>ExpoSKUDelete</t>
   </si>
   <si>
-    <t>Test SKU management in Expoloader  delete.</t>
-  </si>
-  <si>
     <t>Zabith</t>
   </si>
   <si>
     <t>ExpoSKUSearch</t>
   </si>
   <si>
-    <t xml:space="preserve">Test SKU management in Expoloader  Search </t>
-  </si>
-  <si>
     <t>ExpoSKUDeleteAllRecords</t>
   </si>
   <si>
-    <t>Test SKU management in Expoloader  DeleteAllRecords</t>
-  </si>
-  <si>
     <t>ExpoSKUDeleteMultipleRecords</t>
   </si>
   <si>
-    <t xml:space="preserve">Test SKU management to Delete more than one Record in Expoloader  </t>
-  </si>
-  <si>
     <t>ExpoContainerAddNew</t>
   </si>
   <si>
@@ -159,30 +117,18 @@
     <t>ExpoContainerDelete</t>
   </si>
   <si>
-    <t>Test Container management in Expoloader  delete.</t>
-  </si>
-  <si>
     <t>Tisun</t>
   </si>
   <si>
     <t>ExpoContainerSearch</t>
   </si>
   <si>
-    <t xml:space="preserve">Test Containermanagement in Expoloader  Search </t>
-  </si>
-  <si>
     <t>ExpoContainerDeleteAllRecords</t>
   </si>
   <si>
-    <t>Test Containermanagement in Expoloader  DeleteAllRecords</t>
-  </si>
-  <si>
     <t>ExpoPalleteAddNew</t>
   </si>
   <si>
-    <t>Test Pallete management in Expoloader.  AddNew</t>
-  </si>
-  <si>
     <t>ExpoPalleteExportExcel</t>
   </si>
   <si>
@@ -198,30 +144,15 @@
     <t>ExpoPalleteDelete</t>
   </si>
   <si>
-    <t>Test Palletemanagement in Expoloader  delete.</t>
-  </si>
-  <si>
     <t>ExpoPalleteSearch</t>
   </si>
   <si>
-    <t xml:space="preserve">Test Pallete management in Expoloader  Search </t>
-  </si>
-  <si>
     <t>ExpoPalleteDeleteAllRecords</t>
   </si>
   <si>
-    <t>Test Palletemanagement in Expoloader  DeleteAllRecords</t>
-  </si>
-  <si>
     <t>FloorLoading</t>
   </si>
   <si>
-    <t>Test basic container loading  ex-Add LoadingType,Container,Height,SKU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PalletLoading        </t>
-  </si>
-  <si>
     <t>Test basic container loading ex-Add LoadingType,Container,Height,SKU</t>
   </si>
   <si>
@@ -252,81 +183,15 @@
     <t>Check signup Emial verification</t>
   </si>
   <si>
-    <t>Notification</t>
-  </si>
-  <si>
     <t>Test notifications in expoloader website</t>
   </si>
   <si>
-    <t>ForgetPassword</t>
-  </si>
-  <si>
-    <t>Test signin forget password</t>
-  </si>
-  <si>
-    <t>UserProfile</t>
-  </si>
-  <si>
-    <t>Test UserProfile features</t>
-  </si>
-  <si>
-    <t>CreateUpdateSaveFloorLoading</t>
-  </si>
-  <si>
-    <t>test the save load function in floor loading</t>
-  </si>
-  <si>
-    <t>CreateUpdateSavePalletLoading</t>
-  </si>
-  <si>
-    <t>test the save load function in the pallet loading</t>
-  </si>
-  <si>
-    <t>CreateUpdateSavePalletLoadingAndFloorLoading</t>
-  </si>
-  <si>
-    <t>test the save load function in the pallet and floor loading</t>
-  </si>
-  <si>
-    <t>SelectProject</t>
-  </si>
-  <si>
-    <t>test select project function</t>
-  </si>
-  <si>
-    <t>suresh</t>
-  </si>
-  <si>
-    <t>ProjectAdd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test proect Management add </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Suresh </t>
-  </si>
-  <si>
-    <t>ProjectDelete</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test project management delete </t>
-  </si>
-  <si>
     <t>sarfan</t>
   </si>
   <si>
-    <t>ProjectDeleteAllRecords</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test project management delete all </t>
-  </si>
-  <si>
     <t>SearchProject</t>
   </si>
   <si>
-    <t xml:space="preserve">test project  management search </t>
-  </si>
-  <si>
     <t>ProjectDetailsAddUser</t>
   </si>
   <si>
@@ -348,27 +213,15 @@
     <t>test project details Delete user</t>
   </si>
   <si>
-    <t>ConsegmentSearch</t>
-  </si>
-  <si>
     <t>test consegment management's search function</t>
   </si>
   <si>
-    <t>ConsegmentEdit</t>
-  </si>
-  <si>
     <t>test consegment management's edit function</t>
   </si>
   <si>
-    <t>ConsegmentDelete</t>
-  </si>
-  <si>
     <t>test consegment management's delete function</t>
   </si>
   <si>
-    <t>ConsegmentDeleteAllRecords</t>
-  </si>
-  <si>
     <t>test consegment management's DeleteAll function</t>
   </si>
   <si>
@@ -378,15 +231,6 @@
     <t>Developed</t>
   </si>
   <si>
-    <t>ExpoFloorAndPalletLoading</t>
-  </si>
-  <si>
-    <t>Test expoloader floor and pallet loading in the optimization</t>
-  </si>
-  <si>
-    <t>thisun</t>
-  </si>
-  <si>
     <t>PersonalInfo</t>
   </si>
   <si>
@@ -403,6 +247,138 @@
   </si>
   <si>
     <t>test delete account</t>
+  </si>
+  <si>
+    <t>Test SKU management in Expoloader. AddNew</t>
+  </si>
+  <si>
+    <t>Test SKU management in Expoloader delete.</t>
+  </si>
+  <si>
+    <t>Test SKU management in Expoloader Search</t>
+  </si>
+  <si>
+    <t>Test SKU management in Expoloader DeleteAllRecords</t>
+  </si>
+  <si>
+    <t>Test SKU management to Delete more than one Record in Expoloader</t>
+  </si>
+  <si>
+    <t>Test Container management in Expoloader delete.</t>
+  </si>
+  <si>
+    <t>Test Containermanagement in Expoloader Search</t>
+  </si>
+  <si>
+    <t>Test Containermanagement in Expoloader DeleteAllRecords</t>
+  </si>
+  <si>
+    <t>Test Pallete management in Expoloader. AddNew</t>
+  </si>
+  <si>
+    <t>Test Palletemanagement in Expoloader delete.</t>
+  </si>
+  <si>
+    <t>Test Pallete management in Expoloader Search</t>
+  </si>
+  <si>
+    <t>Test Palletemanagement in Expoloader DeleteAllRecords</t>
+  </si>
+  <si>
+    <t>PalletLoading</t>
+  </si>
+  <si>
+    <t>NotificationContainerAddNew</t>
+  </si>
+  <si>
+    <t>Thilina/ayesh/thisun/suresh</t>
+  </si>
+  <si>
+    <t>NotificationContainerDelete</t>
+  </si>
+  <si>
+    <t>NotificationContainerDeleteAllRecord</t>
+  </si>
+  <si>
+    <t>NotificationContainerEdit</t>
+  </si>
+  <si>
+    <t>NotificationPalletAddNew</t>
+  </si>
+  <si>
+    <t>NotificationPalletDelete</t>
+  </si>
+  <si>
+    <t>NotificationPalletDeleteAllRecord</t>
+  </si>
+  <si>
+    <t>NotificationPalletEdit</t>
+  </si>
+  <si>
+    <t>NotificationSKUAddNew</t>
+  </si>
+  <si>
+    <t>NotificationSKUDelete</t>
+  </si>
+  <si>
+    <t>NotificationSKUDeleteAllRecord</t>
+  </si>
+  <si>
+    <t>NotificationSKUEdit</t>
+  </si>
+  <si>
+    <t>NotificationProjectsAddNew</t>
+  </si>
+  <si>
+    <t>NotificationProjectsDelete</t>
+  </si>
+  <si>
+    <t>NotificationProjectsDeleteAllRecord</t>
+  </si>
+  <si>
+    <t>NotificationProjectsEdit</t>
+  </si>
+  <si>
+    <t>NotificationConsignmentsAddNew</t>
+  </si>
+  <si>
+    <t>NotificationConsignmentsDelete</t>
+  </si>
+  <si>
+    <t>NotificationConsignmentsDeleteAllRecords</t>
+  </si>
+  <si>
+    <t>NotificationConsignmentsDeleteEdit</t>
+  </si>
+  <si>
+    <t>NotificationPersonalInfo</t>
+  </si>
+  <si>
+    <t>NotificationDeleteAccount</t>
+  </si>
+  <si>
+    <t>Test Different combination of Username Eg: Empty username,Empty password, Valid Username, Invalid Username,Invalid Password,valid password</t>
+  </si>
+  <si>
+    <t>FloorAndPalletLoading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test floor and pallet loading in the optimization </t>
+  </si>
+  <si>
+    <t>test project management search</t>
+  </si>
+  <si>
+    <t>ConsignmentSearch</t>
+  </si>
+  <si>
+    <t>ConsignmentEdit</t>
+  </si>
+  <si>
+    <t>ConsignmentDelete</t>
+  </si>
+  <si>
+    <t>ConsignmentDeleteAllRecords</t>
   </si>
 </sst>
 </file>
@@ -468,6 +444,8 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -496,7 +474,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -532,27 +510,18 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF9900"/>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF6AA84F"/>
-          <bgColor rgb="FF6AA84F"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="8">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -574,6 +543,14 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFCC0000"/>
           <bgColor rgb="FFCC0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF6AA84F"/>
+          <bgColor rgb="FF6AA84F"/>
         </patternFill>
       </fill>
     </dxf>
@@ -823,10 +800,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AA1017"/>
+  <dimension ref="A1:AA1018"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -858,7 +835,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
@@ -867,16 +844,16 @@
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>109</v>
+        <v>68</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
@@ -889,15 +866,15 @@
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="10" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>12</v>
+        <v>112</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="13" t="s">
@@ -905,341 +882,341 @@
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="10" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>14</v>
+        <v>76</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="10" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="10" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="10" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>21</v>
+        <v>77</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="15" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="10" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>24</v>
+        <v>78</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="15" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="10" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>26</v>
+        <v>79</v>
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="15" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="10" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>28</v>
+        <v>80</v>
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="13"/>
       <c r="E11" s="6"/>
       <c r="F11" s="10" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="13" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="10" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="13" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="10" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C14" s="10"/>
       <c r="D14" s="13" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="10" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>38</v>
+        <v>81</v>
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="13" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="E15" s="6"/>
       <c r="F15" s="10" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A16" s="16" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="13" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="E16" s="6"/>
       <c r="F16" s="10" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A17" s="14" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>43</v>
+        <v>83</v>
       </c>
       <c r="C17" s="10"/>
       <c r="D17" s="13" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="E17" s="6"/>
       <c r="F17" s="10" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>45</v>
+        <v>84</v>
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="16" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E18" s="6"/>
       <c r="F18" s="10" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A19" s="14" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="C19" s="10"/>
       <c r="D19" s="16" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E19" s="6"/>
       <c r="F19" s="10" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A20" s="16" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="C20" s="10"/>
       <c r="D20" s="16" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E20" s="6"/>
       <c r="F20" s="10" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A21" s="16" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>51</v>
+        <v>85</v>
       </c>
       <c r="C21" s="10"/>
       <c r="D21" s="16" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E21" s="6"/>
       <c r="F21" s="10" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A22" s="16" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>53</v>
+        <v>86</v>
       </c>
       <c r="C22" s="10"/>
       <c r="D22" s="16" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E22" s="6"/>
       <c r="F22" s="10" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A23" s="14" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>55</v>
+        <v>87</v>
       </c>
       <c r="C23" s="10"/>
       <c r="D23" s="16" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E23" s="6"/>
       <c r="F23" s="10" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:27" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A24" s="14" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="C24" s="10"/>
       <c r="D24" s="13" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E24" s="6"/>
       <c r="F24" s="10" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:27" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A25" s="17" t="s">
-        <v>58</v>
+        <v>88</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="C25" s="10"/>
       <c r="D25" s="19" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E25" s="6"/>
       <c r="F25" s="10" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
       <c r="G25" s="20"/>
       <c r="H25" s="20"/>
@@ -1264,19 +1241,19 @@
       <c r="AA25" s="20"/>
     </row>
     <row r="26" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A26" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="B26" s="19" t="s">
-        <v>61</v>
+      <c r="A26" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="B26" s="24" t="s">
+        <v>114</v>
       </c>
       <c r="C26" s="10"/>
-      <c r="D26" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="E26" s="6"/>
+      <c r="D26" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="E26" s="10"/>
       <c r="F26" s="10" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
       <c r="G26" s="20"/>
       <c r="H26" s="20"/>
@@ -1302,18 +1279,18 @@
     </row>
     <row r="27" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A27" s="17" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="C27" s="10"/>
       <c r="D27" s="13" t="s">
-        <v>63</v>
+        <v>19</v>
       </c>
       <c r="E27" s="6"/>
       <c r="F27" s="10" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
       <c r="G27" s="20"/>
       <c r="H27" s="20"/>
@@ -1339,18 +1316,18 @@
     </row>
     <row r="28" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A28" s="17" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="C28" s="10"/>
       <c r="D28" s="13" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="E28" s="6"/>
       <c r="F28" s="10" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
       <c r="G28" s="20"/>
       <c r="H28" s="20"/>
@@ -1376,18 +1353,18 @@
     </row>
     <row r="29" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A29" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="B29" s="17" t="s">
-        <v>66</v>
+        <v>49</v>
+      </c>
+      <c r="B29" s="19" t="s">
+        <v>46</v>
       </c>
       <c r="C29" s="10"/>
-      <c r="D29" s="15" t="s">
-        <v>63</v>
+      <c r="D29" s="13" t="s">
+        <v>48</v>
       </c>
       <c r="E29" s="6"/>
       <c r="F29" s="10" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
       <c r="G29" s="20"/>
       <c r="H29" s="20"/>
@@ -1412,307 +1389,328 @@
       <c r="AA29" s="20"/>
     </row>
     <row r="30" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A30" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="B30" s="15" t="s">
-        <v>112</v>
+      <c r="A30" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B30" s="17" t="s">
+        <v>51</v>
       </c>
       <c r="C30" s="10"/>
       <c r="D30" s="15" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="E30" s="6"/>
       <c r="F30" s="10" t="s">
-        <v>110</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
+      <c r="K30" s="20"/>
+      <c r="L30" s="20"/>
+      <c r="M30" s="20"/>
+      <c r="N30" s="20"/>
+      <c r="O30" s="20"/>
+      <c r="P30" s="20"/>
+      <c r="Q30" s="20"/>
+      <c r="R30" s="20"/>
+      <c r="S30" s="20"/>
+      <c r="T30" s="20"/>
+      <c r="U30" s="20"/>
+      <c r="V30" s="20"/>
+      <c r="W30" s="20"/>
+      <c r="X30" s="20"/>
+      <c r="Y30" s="20"/>
+      <c r="Z30" s="20"/>
+      <c r="AA30" s="20"/>
     </row>
     <row r="31" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A31" s="15" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="C31" s="10"/>
       <c r="D31" s="15" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E31" s="6"/>
       <c r="F31" s="10" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
     </row>
     <row r="32" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A32" s="15" t="s">
-        <v>69</v>
+        <v>89</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="C32" s="10"/>
       <c r="D32" s="15" t="s">
-        <v>34</v>
+        <v>90</v>
       </c>
       <c r="E32" s="6"/>
       <c r="F32" s="10" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A33" s="15" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="C33" s="10"/>
       <c r="D33" s="15" t="s">
-        <v>34</v>
+        <v>90</v>
       </c>
       <c r="E33" s="6"/>
       <c r="F33" s="10" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A34" s="15" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="C34" s="10"/>
       <c r="D34" s="15" t="s">
-        <v>15</v>
+        <v>90</v>
       </c>
       <c r="E34" s="6"/>
       <c r="F34" s="10" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A35" s="15" t="s">
-        <v>75</v>
+        <v>93</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="C35" s="10"/>
       <c r="D35" s="15" t="s">
-        <v>22</v>
+        <v>90</v>
       </c>
       <c r="E35" s="6"/>
       <c r="F35" s="10" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A36" s="15" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
       <c r="C36" s="10"/>
       <c r="D36" s="15" t="s">
-        <v>22</v>
+        <v>90</v>
       </c>
       <c r="E36" s="6"/>
       <c r="F36" s="10" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A37" s="15" t="s">
-        <v>79</v>
+        <v>95</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>80</v>
+        <v>54</v>
       </c>
       <c r="C37" s="10"/>
       <c r="D37" s="15" t="s">
-        <v>63</v>
+        <v>90</v>
       </c>
       <c r="E37" s="6"/>
       <c r="F37" s="10" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A38" s="15" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>82</v>
+        <v>54</v>
       </c>
       <c r="C38" s="10"/>
       <c r="D38" s="15" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="E38" s="6"/>
       <c r="F38" s="10" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A39" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="B39" s="21" t="s">
-        <v>85</v>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A39" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>54</v>
       </c>
       <c r="C39" s="10"/>
-      <c r="D39" s="21" t="s">
-        <v>86</v>
+      <c r="D39" s="15" t="s">
+        <v>90</v>
       </c>
       <c r="E39" s="6"/>
       <c r="F39" s="10" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="21" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="B40" s="21" t="s">
-        <v>88</v>
+        <v>54</v>
       </c>
       <c r="C40" s="10"/>
       <c r="D40" s="21" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E40" s="6"/>
       <c r="F40" s="10" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="21" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="B41" s="21" t="s">
-        <v>91</v>
+        <v>54</v>
       </c>
       <c r="C41" s="10"/>
       <c r="D41" s="21" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E41" s="6"/>
       <c r="F41" s="10" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="21" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="B42" s="21" t="s">
-        <v>93</v>
+        <v>54</v>
       </c>
       <c r="C42" s="10"/>
       <c r="D42" s="21" t="s">
-        <v>10</v>
+        <v>90</v>
       </c>
       <c r="E42" s="6"/>
       <c r="F42" s="10" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="21" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="B43" s="21" t="s">
-        <v>95</v>
+        <v>54</v>
       </c>
       <c r="C43" s="10"/>
       <c r="D43" s="21" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="E43" s="6"/>
       <c r="F43" s="10" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="21" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="B44" s="21" t="s">
-        <v>98</v>
+        <v>54</v>
       </c>
       <c r="C44" s="10"/>
       <c r="D44" s="21" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="E44" s="6"/>
       <c r="F44" s="10" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="21" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="B45" s="21" t="s">
-        <v>100</v>
+        <v>54</v>
       </c>
       <c r="C45" s="10"/>
       <c r="D45" s="21" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="E45" s="6"/>
       <c r="F45" s="10" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="21" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B46" s="21" t="s">
-        <v>102</v>
+        <v>54</v>
       </c>
       <c r="C46" s="10"/>
       <c r="D46" s="21" t="s">
-        <v>63</v>
+        <v>90</v>
       </c>
       <c r="E46" s="6"/>
       <c r="F46" s="10" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="21" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B47" s="21" t="s">
-        <v>104</v>
+        <v>54</v>
       </c>
       <c r="C47" s="10"/>
       <c r="D47" s="21" t="s">
-        <v>63</v>
+        <v>90</v>
       </c>
       <c r="E47" s="6"/>
       <c r="F47" s="10" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="21" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B48" s="21" t="s">
-        <v>106</v>
+        <v>54</v>
       </c>
       <c r="C48" s="10"/>
       <c r="D48" s="21" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="E48" s="6"/>
       <c r="F48" s="10" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -1720,124 +1718,256 @@
         <v>107</v>
       </c>
       <c r="B49" s="21" t="s">
-        <v>108</v>
+        <v>54</v>
       </c>
       <c r="C49" s="10"/>
       <c r="D49" s="21" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="E49" s="6"/>
       <c r="F49" s="10" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>114</v>
-      </c>
-      <c r="B50" t="s">
-        <v>115</v>
-      </c>
-      <c r="C50" s="6"/>
-      <c r="D50" t="s">
-        <v>15</v>
+      <c r="A50" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="B50" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="C50" s="10"/>
+      <c r="D50" s="21" t="s">
+        <v>90</v>
       </c>
       <c r="E50" s="6"/>
       <c r="F50" s="10" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B51" t="s">
-        <v>117</v>
+        <v>54</v>
       </c>
       <c r="C51" s="6"/>
       <c r="D51" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E51" s="6"/>
       <c r="F51" s="10" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="B52" t="s">
-        <v>119</v>
+        <v>54</v>
       </c>
       <c r="C52" s="6"/>
       <c r="D52" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E52" s="6"/>
       <c r="F52" s="10" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>111</v>
+      </c>
+      <c r="B53" t="s">
+        <v>54</v>
+      </c>
       <c r="C53" s="6"/>
+      <c r="D53" t="s">
+        <v>90</v>
+      </c>
       <c r="E53" s="6"/>
-      <c r="F53" s="6"/>
+      <c r="F53" s="10" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="54" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>56</v>
+      </c>
+      <c r="B54" t="s">
+        <v>115</v>
+      </c>
       <c r="C54" s="6"/>
+      <c r="D54" t="s">
+        <v>10</v>
+      </c>
       <c r="E54" s="6"/>
-      <c r="F54" s="6"/>
+      <c r="F54" s="10" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="55" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>57</v>
+      </c>
+      <c r="B55" t="s">
+        <v>58</v>
+      </c>
       <c r="C55" s="6"/>
+      <c r="D55" t="s">
+        <v>19</v>
+      </c>
       <c r="E55" s="6"/>
-      <c r="F55" s="6"/>
+      <c r="F55" s="10" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="56" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>60</v>
+      </c>
+      <c r="B56" t="s">
+        <v>61</v>
+      </c>
       <c r="C56" s="6"/>
+      <c r="D56" t="s">
+        <v>19</v>
+      </c>
       <c r="E56" s="6"/>
-      <c r="F56" s="6"/>
+      <c r="F56" s="10" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="57" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>62</v>
+      </c>
+      <c r="B57" t="s">
+        <v>63</v>
+      </c>
       <c r="C57" s="6"/>
+      <c r="D57" t="s">
+        <v>19</v>
+      </c>
       <c r="E57" s="6"/>
-      <c r="F57" s="6"/>
+      <c r="F57" s="10" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="58" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>116</v>
+      </c>
+      <c r="B58" t="s">
+        <v>64</v>
+      </c>
       <c r="C58" s="6"/>
+      <c r="D58" t="s">
+        <v>48</v>
+      </c>
       <c r="E58" s="6"/>
-      <c r="F58" s="6"/>
+      <c r="F58" s="10" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="59" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>117</v>
+      </c>
+      <c r="B59" t="s">
+        <v>65</v>
+      </c>
       <c r="C59" s="6"/>
+      <c r="D59" t="s">
+        <v>48</v>
+      </c>
       <c r="E59" s="6"/>
-      <c r="F59" s="6"/>
+      <c r="F59" s="10" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="60" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>118</v>
+      </c>
+      <c r="B60" t="s">
+        <v>66</v>
+      </c>
       <c r="C60" s="6"/>
+      <c r="D60" t="s">
+        <v>59</v>
+      </c>
       <c r="E60" s="6"/>
-      <c r="F60" s="6"/>
+      <c r="F60" s="10" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="61" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>119</v>
+      </c>
+      <c r="B61" t="s">
+        <v>67</v>
+      </c>
       <c r="C61" s="6"/>
+      <c r="D61" t="s">
+        <v>59</v>
+      </c>
       <c r="E61" s="6"/>
-      <c r="F61" s="6"/>
+      <c r="F61" s="10" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="62" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>70</v>
+      </c>
+      <c r="B62" t="s">
+        <v>71</v>
+      </c>
       <c r="C62" s="6"/>
+      <c r="D62" t="s">
+        <v>13</v>
+      </c>
       <c r="E62" s="6"/>
-      <c r="F62" s="6"/>
+      <c r="F62" s="10" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="63" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>72</v>
+      </c>
+      <c r="B63" t="s">
+        <v>73</v>
+      </c>
       <c r="C63" s="6"/>
+      <c r="D63" t="s">
+        <v>55</v>
+      </c>
       <c r="E63" s="6"/>
-      <c r="F63" s="6"/>
+      <c r="F63" s="10" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="64" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>74</v>
+      </c>
+      <c r="B64" t="s">
+        <v>75</v>
+      </c>
       <c r="C64" s="6"/>
+      <c r="D64" t="s">
+        <v>55</v>
+      </c>
       <c r="E64" s="6"/>
-      <c r="F64" s="6"/>
+      <c r="F64" s="10" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="65" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C65" s="6"/>
@@ -6520,8 +6650,9 @@
       <c r="F1000" s="6"/>
     </row>
     <row r="1001" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="E1001" s="22"/>
-      <c r="F1001" s="22"/>
+      <c r="C1001" s="6"/>
+      <c r="E1001" s="6"/>
+      <c r="F1001" s="6"/>
     </row>
     <row r="1002" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="E1002" s="22"/>
@@ -6587,44 +6718,40 @@
       <c r="E1017" s="22"/>
       <c r="F1017" s="22"/>
     </row>
+    <row r="1018" spans="5:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="E1018" s="22"/>
+      <c r="F1018" s="22"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="F2:F1017">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+  <conditionalFormatting sqref="F2:F1018">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"Developed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F1017">
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+  <conditionalFormatting sqref="E2:F1018">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E1017">
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+  <conditionalFormatting sqref="E2:E1018">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"Tested"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E1017">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
-      <formula>"Pending"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E1017">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+  <conditionalFormatting sqref="E2:E1018">
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
       <formula>"Issue"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" sqref="F2:F1017">
+    <dataValidation type="list" allowBlank="1" sqref="F2:F1018">
       <formula1>"Developed,Pending"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="E2:E1017">
+    <dataValidation type="list" allowBlank="1" sqref="E2:E1018">
       <formula1>"Tested,Pending,Issue"</formula1>
     </dataValidation>
   </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
expoSKUDelete, expoSKUDeleteAllRecords, expoSKUSearch, expoPalletEdit, expoPalletAddNew, navExpoloader
</commit_message>
<xml_diff>
--- a/tests/TestCasesPlan.xlsx
+++ b/tests/TestCasesPlan.xlsx
@@ -390,10 +390,10 @@
     <t>SKU import excel data</t>
   </si>
   <si>
-    <t>ExpoPalletImportExcelData</t>
-  </si>
-  <si>
-    <t>pallet import excel data</t>
+    <t>ExpoPalleteImportExcel</t>
+  </si>
+  <si>
+    <t>container export excel data</t>
   </si>
 </sst>
 </file>
@@ -785,8 +785,8 @@
   </sheetPr>
   <dimension ref="A1:AA1020"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1116,7 +1116,7 @@
     </row>
     <row r="20" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A20" s="14" t="s">
-        <v>35</v>
+        <v>123</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>36</v>
@@ -1196,7 +1196,7 @@
     </row>
     <row r="25" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A25" s="17" t="s">
-        <v>123</v>
+        <v>35</v>
       </c>
       <c r="B25" s="9" t="s">
         <v>124</v>

</xml_diff>

<commit_message>
Updated test case plan
</commit_message>
<xml_diff>
--- a/tests/TestCasesPlan.xlsx
+++ b/tests/TestCasesPlan.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="133">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -39,123 +39,54 @@
     <t>Developers Status</t>
   </si>
   <si>
-    <t>NavExpo</t>
-  </si>
-  <si>
     <t>Navigate the URL</t>
   </si>
   <si>
-    <t>SignupExpo</t>
-  </si>
-  <si>
     <t>Test Different combination of Username value. Eg: Empty username,Empty password,Empty Email, Valid Username, Invalid Username,Invalid Email,invalid password, valid password, Empty Check Box</t>
   </si>
   <si>
     <t>Suresh</t>
   </si>
   <si>
-    <t>LoginExpo</t>
-  </si>
-  <si>
-    <t>ExpoSKUAddNew</t>
-  </si>
-  <si>
     <t>Amna</t>
   </si>
   <si>
-    <t>ExpoSKUIExportExcel</t>
-  </si>
-  <si>
     <t>Test SKU management in Expoloader ImportExel</t>
   </si>
   <si>
-    <t>ExpoSKUEdit</t>
-  </si>
-  <si>
     <t>Test SKU management in Expoloader edit</t>
   </si>
   <si>
-    <t>ExpoSKUDelete</t>
-  </si>
-  <si>
     <t>Zabith</t>
   </si>
   <si>
-    <t>ExpoSKUSearch</t>
-  </si>
-  <si>
-    <t>ExpoSKUDeleteAllRecords</t>
-  </si>
-  <si>
-    <t>ExpoContainerAddNew</t>
-  </si>
-  <si>
     <t>Test Container management in Expoloader AddNew</t>
   </si>
   <si>
     <t>Thilina/thisun</t>
   </si>
   <si>
-    <t>ExpoContainerExportExcel</t>
-  </si>
-  <si>
     <t>Test Container management in Expoloader ImportExel</t>
   </si>
   <si>
     <t>Thilina</t>
   </si>
   <si>
-    <t>ExpoContainerEdit</t>
-  </si>
-  <si>
     <t>Test Container management in Expoloader edit</t>
   </si>
   <si>
-    <t>ExpoContainerDelete</t>
-  </si>
-  <si>
     <t>Tisun</t>
   </si>
   <si>
-    <t>ExpoContainerSearch</t>
-  </si>
-  <si>
-    <t>ExpoContainerDeleteAllRecords</t>
-  </si>
-  <si>
-    <t>ExpoPalleteAddNew</t>
-  </si>
-  <si>
-    <t>ExpoPalleteExportExcel</t>
-  </si>
-  <si>
     <t>Test Pallete management in Expoloader ImportExel</t>
   </si>
   <si>
-    <t>ExpoPalleteEdit</t>
-  </si>
-  <si>
     <t>Test Palletemanagement in Expoloader edit</t>
   </si>
   <si>
-    <t>ExpoPalleteDelete</t>
-  </si>
-  <si>
-    <t>ExpoPalleteSearch</t>
-  </si>
-  <si>
-    <t>ExpoPalleteDeleteAllRecords</t>
-  </si>
-  <si>
-    <t>FloorLoading</t>
-  </si>
-  <si>
     <t>Test basic container loading ex-Add LoadingType,Container,Height,SKU</t>
   </si>
   <si>
-    <t>MultiSkuFloorLoading</t>
-  </si>
-  <si>
     <t>Test multiple sku</t>
   </si>
   <si>
@@ -168,15 +99,9 @@
     <t>palletNonStackMultiSkuLoad</t>
   </si>
   <si>
-    <t>LogOut</t>
-  </si>
-  <si>
     <t>Logout of the website</t>
   </si>
   <si>
-    <t>Email Verification</t>
-  </si>
-  <si>
     <t>Check signup Emial verification</t>
   </si>
   <si>
@@ -186,27 +111,15 @@
     <t>sarfan</t>
   </si>
   <si>
-    <t>SearchProject</t>
-  </si>
-  <si>
-    <t>ProjectDetailsAddUser</t>
-  </si>
-  <si>
     <t>test project details add user</t>
   </si>
   <si>
     <t>Navindu</t>
   </si>
   <si>
-    <t>ProjectDetailsEdit</t>
-  </si>
-  <si>
     <t>test project details Edit</t>
   </si>
   <si>
-    <t>ProjectDetailsDelete</t>
-  </si>
-  <si>
     <t>test project details Delete user</t>
   </si>
   <si>
@@ -228,21 +141,12 @@
     <t>Developed</t>
   </si>
   <si>
-    <t>PersonalInfo</t>
-  </si>
-  <si>
     <t>test personal Info</t>
   </si>
   <si>
-    <t>ChangePassword</t>
-  </si>
-  <si>
     <t>test change password function</t>
   </si>
   <si>
-    <t>DeleteAccount</t>
-  </si>
-  <si>
     <t>test delete account</t>
   </si>
   <si>
@@ -279,132 +183,259 @@
     <t>Test Palletemanagement in Expoloader DeleteAllRecords</t>
   </si>
   <si>
-    <t>PalletLoading</t>
-  </si>
-  <si>
-    <t>NotificationContainerAddNew</t>
-  </si>
-  <si>
     <t>Thilina/ayesh/thisun/suresh</t>
   </si>
   <si>
-    <t>NotificationContainerDelete</t>
-  </si>
-  <si>
-    <t>NotificationContainerDeleteAllRecord</t>
-  </si>
-  <si>
-    <t>NotificationContainerEdit</t>
-  </si>
-  <si>
-    <t>NotificationPalletAddNew</t>
-  </si>
-  <si>
-    <t>NotificationPalletDelete</t>
-  </si>
-  <si>
-    <t>NotificationPalletDeleteAllRecord</t>
-  </si>
-  <si>
-    <t>NotificationPalletEdit</t>
-  </si>
-  <si>
-    <t>NotificationSKUAddNew</t>
-  </si>
-  <si>
-    <t>NotificationSKUDelete</t>
-  </si>
-  <si>
-    <t>NotificationSKUDeleteAllRecord</t>
-  </si>
-  <si>
-    <t>NotificationSKUEdit</t>
-  </si>
-  <si>
-    <t>NotificationProjectsAddNew</t>
-  </si>
-  <si>
-    <t>NotificationProjectsDelete</t>
-  </si>
-  <si>
-    <t>NotificationProjectsDeleteAllRecord</t>
-  </si>
-  <si>
-    <t>NotificationProjectsEdit</t>
-  </si>
-  <si>
-    <t>NotificationConsignmentsAddNew</t>
-  </si>
-  <si>
-    <t>NotificationConsignmentsDelete</t>
-  </si>
-  <si>
-    <t>NotificationConsignmentsDeleteAllRecords</t>
-  </si>
-  <si>
-    <t>NotificationConsignmentsDeleteEdit</t>
-  </si>
-  <si>
-    <t>NotificationPersonalInfo</t>
-  </si>
-  <si>
-    <t>NotificationDeleteAccount</t>
-  </si>
-  <si>
     <t>Test Different combination of Username Eg: Empty username,Empty password, Valid Username, Invalid Username,Invalid Password,valid password</t>
   </si>
   <si>
-    <t>FloorAndPalletLoading</t>
-  </si>
-  <si>
     <t xml:space="preserve">test floor and pallet loading in the optimization </t>
   </si>
   <si>
     <t>test project management search</t>
   </si>
   <si>
-    <t>ConsignmentSearch</t>
-  </si>
-  <si>
-    <t>ConsignmentEdit</t>
-  </si>
-  <si>
-    <t>ConsignmentDelete</t>
-  </si>
-  <si>
-    <t>ConsignmentDeleteAllRecords</t>
-  </si>
-  <si>
-    <t>Thisun</t>
-  </si>
-  <si>
-    <t>ExpoSKUImportExcelData</t>
-  </si>
-  <si>
-    <t>ExpoContainerImportExcelData</t>
-  </si>
-  <si>
     <t>container import excel data</t>
   </si>
   <si>
     <t>SKU import excel data</t>
   </si>
   <si>
-    <t>ExpoPalleteImportExcel</t>
-  </si>
-  <si>
     <t>container export excel data</t>
+  </si>
+  <si>
+    <t>test project add</t>
+  </si>
+  <si>
+    <t>thisun</t>
+  </si>
+  <si>
+    <t>test project Edit</t>
+  </si>
+  <si>
+    <t>test project Delete</t>
+  </si>
+  <si>
+    <t>test project delete all records</t>
+  </si>
+  <si>
+    <t>expoSKUDeleteAllRecords</t>
+  </si>
+  <si>
+    <t>expoSKUSearch</t>
+  </si>
+  <si>
+    <t>expoSKUDelete</t>
+  </si>
+  <si>
+    <t>expoSKUEdit</t>
+  </si>
+  <si>
+    <t>expoSKUIExportExcel</t>
+  </si>
+  <si>
+    <t>expoSKUAddNew</t>
+  </si>
+  <si>
+    <t>loginExpo</t>
+  </si>
+  <si>
+    <t>expoSKUImportExcelData</t>
+  </si>
+  <si>
+    <t>expoContainerAddNew</t>
+  </si>
+  <si>
+    <t>expoContainerExportExcel</t>
+  </si>
+  <si>
+    <t>expoContainerEdit</t>
+  </si>
+  <si>
+    <t>expoContainerDelete</t>
+  </si>
+  <si>
+    <t>expoContainerSearch</t>
+  </si>
+  <si>
+    <t>expoContainerDeleteAllRecords</t>
+  </si>
+  <si>
+    <t>expoContainerImportExcelData</t>
+  </si>
+  <si>
+    <t>expoPalleteAddNew</t>
+  </si>
+  <si>
+    <t>expoPalleteImportExcel</t>
+  </si>
+  <si>
+    <t>expoPalleteEdit</t>
+  </si>
+  <si>
+    <t>expoPalleteDelete</t>
+  </si>
+  <si>
+    <t>expoPalleteSearch</t>
+  </si>
+  <si>
+    <t>expoPalleteDeleteAllRecords</t>
+  </si>
+  <si>
+    <t>expoPalleteExportExcel</t>
+  </si>
+  <si>
+    <t>floorLoading</t>
+  </si>
+  <si>
+    <t>palletLoading</t>
+  </si>
+  <si>
+    <t>floorAndPalletLoading</t>
+  </si>
+  <si>
+    <t>multiSkuFloorLoading</t>
+  </si>
+  <si>
+    <t>logOut</t>
+  </si>
+  <si>
+    <t>email Verification</t>
+  </si>
+  <si>
+    <t>notificationContainerAddNew</t>
+  </si>
+  <si>
+    <t>notificationContainerDelete</t>
+  </si>
+  <si>
+    <t>notificationContainerDeleteAllRecord</t>
+  </si>
+  <si>
+    <t>notificationContainerEdit</t>
+  </si>
+  <si>
+    <t>notificationPalletAddNew</t>
+  </si>
+  <si>
+    <t>notificationPalletDelete</t>
+  </si>
+  <si>
+    <t>notificationPalletDeleteAllRecord</t>
+  </si>
+  <si>
+    <t>notificationPalletEdit</t>
+  </si>
+  <si>
+    <t>notificationSKUAddNew</t>
+  </si>
+  <si>
+    <t>notificationSKUDelete</t>
+  </si>
+  <si>
+    <t>notificationSKUDeleteAllRecord</t>
+  </si>
+  <si>
+    <t>notificationSKUEdit</t>
+  </si>
+  <si>
+    <t>notificationProjectsAddNew</t>
+  </si>
+  <si>
+    <t>notificationProjectsDelete</t>
+  </si>
+  <si>
+    <t>notificationProjectsDeleteAllRecord</t>
+  </si>
+  <si>
+    <t>notificationProjectsEdit</t>
+  </si>
+  <si>
+    <t>notificationConsignmentsAddNew</t>
+  </si>
+  <si>
+    <t>notificationConsignmentsDelete</t>
+  </si>
+  <si>
+    <t>notificationConsignmentsDeleteAllRecords</t>
+  </si>
+  <si>
+    <t>notificationConsignmentsDeleteEdit</t>
+  </si>
+  <si>
+    <t>notificationPersonalInfo</t>
+  </si>
+  <si>
+    <t>notificationDeleteAccount</t>
+  </si>
+  <si>
+    <t>searchProject</t>
+  </si>
+  <si>
+    <t>projectAdd</t>
+  </si>
+  <si>
+    <t>projectEdit</t>
+  </si>
+  <si>
+    <t>projectDelete</t>
+  </si>
+  <si>
+    <t>projectDeleteAllRecords</t>
+  </si>
+  <si>
+    <t>projectDetailsAddUser</t>
+  </si>
+  <si>
+    <t>projectDetailsEdit</t>
+  </si>
+  <si>
+    <t>projectDetailsDelete</t>
+  </si>
+  <si>
+    <t>consignmentSearch</t>
+  </si>
+  <si>
+    <t>consignmentEdit</t>
+  </si>
+  <si>
+    <t>consignmentDelete</t>
+  </si>
+  <si>
+    <t>consignmentDeleteAllRecords</t>
+  </si>
+  <si>
+    <t>personalInfo</t>
+  </si>
+  <si>
+    <t>changePassword</t>
+  </si>
+  <si>
+    <t>deleteAccount</t>
+  </si>
+  <si>
+    <t>signupExpo</t>
+  </si>
+  <si>
+    <t>navExpoloader</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -462,6 +493,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -489,54 +534,139 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="14">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF9900"/>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF6AA84F"/>
+          <bgColor rgb="FF6AA84F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCC0000"/>
+          <bgColor rgb="FFCC0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF6AA84F"/>
+          <bgColor rgb="FF6AA84F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF9900"/>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF6AA84F"/>
+          <bgColor rgb="FF6AA84F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCC0000"/>
+          <bgColor rgb="FFCC0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF6AA84F"/>
+          <bgColor rgb="FF6AA84F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF9900"/>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF6AA84F"/>
+          <bgColor rgb="FF6AA84F"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -783,10 +913,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AA1020"/>
+  <dimension ref="A1:AA1024"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -819,1198 +949,1246 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>6</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>7</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="7" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>67</v>
+        <v>38</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="71.25" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
-        <v>8</v>
+      <c r="A3" s="22" t="s">
+        <v>131</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="10" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
-        <v>11</v>
+      <c r="A4" s="22" t="s">
+        <v>72</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="13" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="10" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A5" s="14" t="s">
-        <v>12</v>
+      <c r="A5" s="22" t="s">
+        <v>71</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>75</v>
+        <v>43</v>
       </c>
       <c r="C5" s="10"/>
-      <c r="D5" s="15" t="s">
-        <v>13</v>
+      <c r="D5" s="14" t="s">
+        <v>9</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="10" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="14" t="s">
-        <v>14</v>
+      <c r="A6" s="22" t="s">
+        <v>70</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C6" s="10"/>
-      <c r="D6" s="15" t="s">
-        <v>13</v>
+      <c r="D6" s="14" t="s">
+        <v>9</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="10" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A7" s="16" t="s">
-        <v>16</v>
+      <c r="A7" s="26" t="s">
+        <v>69</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C7" s="10"/>
-      <c r="D7" s="15" t="s">
-        <v>13</v>
+      <c r="D7" s="14" t="s">
+        <v>9</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A8" s="26" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A8" s="16" t="s">
-        <v>18</v>
-      </c>
       <c r="B8" s="9" t="s">
-        <v>76</v>
+        <v>44</v>
       </c>
       <c r="C8" s="10"/>
-      <c r="D8" s="15" t="s">
-        <v>19</v>
+      <c r="D8" s="14" t="s">
+        <v>12</v>
       </c>
       <c r="E8" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A9" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="F8" s="10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A9" s="16" t="s">
-        <v>20</v>
-      </c>
       <c r="B9" s="9" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
       <c r="C9" s="10"/>
-      <c r="D9" s="15" t="s">
-        <v>19</v>
+      <c r="D9" s="14" t="s">
+        <v>12</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>67</v>
+        <v>38</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A10" s="16" t="s">
-        <v>21</v>
+      <c r="A10" s="26" t="s">
+        <v>66</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>78</v>
+        <v>46</v>
       </c>
       <c r="C10" s="10"/>
-      <c r="D10" s="15" t="s">
-        <v>19</v>
+      <c r="D10" s="14" t="s">
+        <v>12</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>67</v>
+        <v>38</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A11" s="16" t="s">
-        <v>119</v>
+      <c r="A11" s="26" t="s">
+        <v>73</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>122</v>
+        <v>59</v>
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="13" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="10" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="14" t="s">
-        <v>22</v>
+      <c r="A12" s="22" t="s">
+        <v>74</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="13" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="10" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A13" s="14" t="s">
-        <v>25</v>
+      <c r="A13" s="22" t="s">
+        <v>75</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="13" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="10" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A14" s="16" t="s">
-        <v>28</v>
+      <c r="A14" s="26" t="s">
+        <v>76</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="C14" s="10"/>
       <c r="D14" s="13" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="10" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A15" s="16" t="s">
-        <v>30</v>
+      <c r="A15" s="26" t="s">
+        <v>77</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="13" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="E15" s="6"/>
       <c r="F15" s="10" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A16" s="16" t="s">
-        <v>32</v>
+      <c r="A16" s="26" t="s">
+        <v>78</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>80</v>
+        <v>48</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="13" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="E16" s="6"/>
       <c r="F16" s="10" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:27" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A17" s="14" t="s">
-        <v>33</v>
+      <c r="A17" s="22" t="s">
+        <v>79</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>81</v>
+        <v>49</v>
       </c>
       <c r="C17" s="10"/>
       <c r="D17" s="13" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="E17" s="6"/>
       <c r="F17" s="10" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A18" s="17" t="s">
-        <v>120</v>
+      <c r="A18" s="22" t="s">
+        <v>80</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>121</v>
+        <v>58</v>
       </c>
       <c r="C18" s="10"/>
-      <c r="D18" s="15" t="s">
-        <v>19</v>
+      <c r="D18" s="14" t="s">
+        <v>12</v>
       </c>
       <c r="E18" s="10"/>
       <c r="F18" s="10" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A19" s="14" t="s">
-        <v>34</v>
+      <c r="A19" s="22" t="s">
+        <v>81</v>
       </c>
       <c r="B19" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="10"/>
+      <c r="D19" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A20" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="16" t="s">
+      <c r="B20" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E19" s="6"/>
-      <c r="F19" s="10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="20" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A20" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>36</v>
-      </c>
       <c r="C20" s="10"/>
-      <c r="D20" s="16" t="s">
-        <v>19</v>
+      <c r="D20" s="15" t="s">
+        <v>12</v>
       </c>
       <c r="E20" s="6"/>
       <c r="F20" s="10" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A21" s="16" t="s">
-        <v>37</v>
+      <c r="A21" s="26" t="s">
+        <v>83</v>
       </c>
       <c r="B21" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="10"/>
+      <c r="D21" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C21" s="10"/>
-      <c r="D21" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="E21" s="6"/>
       <c r="F21" s="10" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A22" s="16" t="s">
-        <v>39</v>
+      <c r="A22" s="26" t="s">
+        <v>84</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>83</v>
+        <v>51</v>
       </c>
       <c r="C22" s="10"/>
-      <c r="D22" s="16" t="s">
-        <v>19</v>
+      <c r="D22" s="15" t="s">
+        <v>12</v>
       </c>
       <c r="E22" s="6"/>
       <c r="F22" s="10" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A23" s="16" t="s">
-        <v>40</v>
+      <c r="A23" s="26" t="s">
+        <v>85</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>84</v>
+        <v>52</v>
       </c>
       <c r="C23" s="10"/>
-      <c r="D23" s="16" t="s">
-        <v>19</v>
+      <c r="D23" s="15" t="s">
+        <v>12</v>
       </c>
       <c r="E23" s="6"/>
       <c r="F23" s="10" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:27" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A24" s="14" t="s">
-        <v>41</v>
+      <c r="A24" s="22" t="s">
+        <v>86</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="C24" s="10"/>
-      <c r="D24" s="16" t="s">
-        <v>19</v>
+      <c r="D24" s="15" t="s">
+        <v>12</v>
       </c>
       <c r="E24" s="6"/>
       <c r="F24" s="10" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A25" s="17" t="s">
-        <v>35</v>
+      <c r="A25" s="22" t="s">
+        <v>87</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>124</v>
+        <v>60</v>
       </c>
       <c r="C25" s="10"/>
-      <c r="D25" s="16" t="s">
-        <v>19</v>
+      <c r="D25" s="15" t="s">
+        <v>12</v>
       </c>
       <c r="E25" s="10"/>
       <c r="F25" s="10" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:27" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A26" s="14" t="s">
-        <v>42</v>
+      <c r="A26" s="22" t="s">
+        <v>88</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="C26" s="10"/>
       <c r="D26" s="13" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E26" s="6"/>
       <c r="F26" s="10" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:27" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A27" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="B27" s="18" t="s">
-        <v>43</v>
+      <c r="A27" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="B27" s="17" t="s">
+        <v>21</v>
       </c>
       <c r="C27" s="10"/>
-      <c r="D27" s="19" t="s">
-        <v>13</v>
+      <c r="D27" s="18" t="s">
+        <v>9</v>
       </c>
       <c r="E27" s="6"/>
       <c r="F27" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20"/>
-      <c r="I27" s="20"/>
-      <c r="J27" s="20"/>
-      <c r="K27" s="20"/>
-      <c r="L27" s="20"/>
-      <c r="M27" s="20"/>
-      <c r="N27" s="20"/>
-      <c r="O27" s="20"/>
-      <c r="P27" s="20"/>
-      <c r="Q27" s="20"/>
-      <c r="R27" s="20"/>
-      <c r="S27" s="20"/>
-      <c r="T27" s="20"/>
-      <c r="U27" s="20"/>
-      <c r="V27" s="20"/>
-      <c r="W27" s="20"/>
-      <c r="X27" s="20"/>
-      <c r="Y27" s="20"/>
-      <c r="Z27" s="20"/>
-      <c r="AA27" s="20"/>
+        <v>39</v>
+      </c>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="19"/>
+      <c r="J27" s="19"/>
+      <c r="K27" s="19"/>
+      <c r="L27" s="19"/>
+      <c r="M27" s="19"/>
+      <c r="N27" s="19"/>
+      <c r="O27" s="19"/>
+      <c r="P27" s="19"/>
+      <c r="Q27" s="19"/>
+      <c r="R27" s="19"/>
+      <c r="S27" s="19"/>
+      <c r="T27" s="19"/>
+      <c r="U27" s="19"/>
+      <c r="V27" s="19"/>
+      <c r="W27" s="19"/>
+      <c r="X27" s="19"/>
+      <c r="Y27" s="19"/>
+      <c r="Z27" s="19"/>
+      <c r="AA27" s="19"/>
     </row>
     <row r="28" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A28" s="23" t="s">
-        <v>111</v>
-      </c>
-      <c r="B28" s="24" t="s">
-        <v>112</v>
+      <c r="A28" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="B28" s="23" t="s">
+        <v>56</v>
       </c>
       <c r="C28" s="10"/>
-      <c r="D28" s="25" t="s">
-        <v>47</v>
+      <c r="D28" s="24" t="s">
+        <v>24</v>
       </c>
       <c r="E28" s="10"/>
       <c r="F28" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="G28" s="20"/>
-      <c r="H28" s="20"/>
-      <c r="I28" s="20"/>
-      <c r="J28" s="20"/>
-      <c r="K28" s="20"/>
-      <c r="L28" s="20"/>
-      <c r="M28" s="20"/>
-      <c r="N28" s="20"/>
-      <c r="O28" s="20"/>
-      <c r="P28" s="20"/>
-      <c r="Q28" s="20"/>
-      <c r="R28" s="20"/>
-      <c r="S28" s="20"/>
-      <c r="T28" s="20"/>
-      <c r="U28" s="20"/>
-      <c r="V28" s="20"/>
-      <c r="W28" s="20"/>
-      <c r="X28" s="20"/>
-      <c r="Y28" s="20"/>
-      <c r="Z28" s="20"/>
-      <c r="AA28" s="20"/>
+        <v>39</v>
+      </c>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
+      <c r="K28" s="19"/>
+      <c r="L28" s="19"/>
+      <c r="M28" s="19"/>
+      <c r="N28" s="19"/>
+      <c r="O28" s="19"/>
+      <c r="P28" s="19"/>
+      <c r="Q28" s="19"/>
+      <c r="R28" s="19"/>
+      <c r="S28" s="19"/>
+      <c r="T28" s="19"/>
+      <c r="U28" s="19"/>
+      <c r="V28" s="19"/>
+      <c r="W28" s="19"/>
+      <c r="X28" s="19"/>
+      <c r="Y28" s="19"/>
+      <c r="Z28" s="19"/>
+      <c r="AA28" s="19"/>
     </row>
     <row r="29" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A29" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="B29" s="19" t="s">
-        <v>45</v>
+      <c r="A29" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="B29" s="18" t="s">
+        <v>22</v>
       </c>
       <c r="C29" s="10"/>
       <c r="D29" s="13" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E29" s="6"/>
       <c r="F29" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="G29" s="20"/>
-      <c r="H29" s="20"/>
-      <c r="I29" s="20"/>
-      <c r="J29" s="20"/>
-      <c r="K29" s="20"/>
-      <c r="L29" s="20"/>
-      <c r="M29" s="20"/>
-      <c r="N29" s="20"/>
-      <c r="O29" s="20"/>
-      <c r="P29" s="20"/>
-      <c r="Q29" s="20"/>
-      <c r="R29" s="20"/>
-      <c r="S29" s="20"/>
-      <c r="T29" s="20"/>
-      <c r="U29" s="20"/>
-      <c r="V29" s="20"/>
-      <c r="W29" s="20"/>
-      <c r="X29" s="20"/>
-      <c r="Y29" s="20"/>
-      <c r="Z29" s="20"/>
-      <c r="AA29" s="20"/>
+        <v>39</v>
+      </c>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="19"/>
+      <c r="K29" s="19"/>
+      <c r="L29" s="19"/>
+      <c r="M29" s="19"/>
+      <c r="N29" s="19"/>
+      <c r="O29" s="19"/>
+      <c r="P29" s="19"/>
+      <c r="Q29" s="19"/>
+      <c r="R29" s="19"/>
+      <c r="S29" s="19"/>
+      <c r="T29" s="19"/>
+      <c r="U29" s="19"/>
+      <c r="V29" s="19"/>
+      <c r="W29" s="19"/>
+      <c r="X29" s="19"/>
+      <c r="Y29" s="19"/>
+      <c r="Z29" s="19"/>
+      <c r="AA29" s="19"/>
     </row>
     <row r="30" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A30" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="B30" s="19" t="s">
-        <v>45</v>
+      <c r="A30" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" s="18" t="s">
+        <v>22</v>
       </c>
       <c r="C30" s="10"/>
       <c r="D30" s="13" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="E30" s="6"/>
       <c r="F30" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
-      <c r="K30" s="20"/>
-      <c r="L30" s="20"/>
-      <c r="M30" s="20"/>
-      <c r="N30" s="20"/>
-      <c r="O30" s="20"/>
-      <c r="P30" s="20"/>
-      <c r="Q30" s="20"/>
-      <c r="R30" s="20"/>
-      <c r="S30" s="20"/>
-      <c r="T30" s="20"/>
-      <c r="U30" s="20"/>
-      <c r="V30" s="20"/>
-      <c r="W30" s="20"/>
-      <c r="X30" s="20"/>
-      <c r="Y30" s="20"/>
-      <c r="Z30" s="20"/>
-      <c r="AA30" s="20"/>
+        <v>39</v>
+      </c>
+      <c r="G30" s="19"/>
+      <c r="H30" s="19"/>
+      <c r="I30" s="19"/>
+      <c r="J30" s="19"/>
+      <c r="K30" s="19"/>
+      <c r="L30" s="19"/>
+      <c r="M30" s="19"/>
+      <c r="N30" s="19"/>
+      <c r="O30" s="19"/>
+      <c r="P30" s="19"/>
+      <c r="Q30" s="19"/>
+      <c r="R30" s="19"/>
+      <c r="S30" s="19"/>
+      <c r="T30" s="19"/>
+      <c r="U30" s="19"/>
+      <c r="V30" s="19"/>
+      <c r="W30" s="19"/>
+      <c r="X30" s="19"/>
+      <c r="Y30" s="19"/>
+      <c r="Z30" s="19"/>
+      <c r="AA30" s="19"/>
     </row>
     <row r="31" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A31" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="B31" s="19" t="s">
-        <v>45</v>
+      <c r="A31" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B31" s="18" t="s">
+        <v>22</v>
       </c>
       <c r="C31" s="10"/>
       <c r="D31" s="13" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="E31" s="6"/>
       <c r="F31" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="G31" s="20"/>
-      <c r="H31" s="20"/>
-      <c r="I31" s="20"/>
-      <c r="J31" s="20"/>
-      <c r="K31" s="20"/>
-      <c r="L31" s="20"/>
-      <c r="M31" s="20"/>
-      <c r="N31" s="20"/>
-      <c r="O31" s="20"/>
-      <c r="P31" s="20"/>
-      <c r="Q31" s="20"/>
-      <c r="R31" s="20"/>
-      <c r="S31" s="20"/>
-      <c r="T31" s="20"/>
-      <c r="U31" s="20"/>
-      <c r="V31" s="20"/>
-      <c r="W31" s="20"/>
-      <c r="X31" s="20"/>
-      <c r="Y31" s="20"/>
-      <c r="Z31" s="20"/>
-      <c r="AA31" s="20"/>
+        <v>39</v>
+      </c>
+      <c r="G31" s="19"/>
+      <c r="H31" s="19"/>
+      <c r="I31" s="19"/>
+      <c r="J31" s="19"/>
+      <c r="K31" s="19"/>
+      <c r="L31" s="19"/>
+      <c r="M31" s="19"/>
+      <c r="N31" s="19"/>
+      <c r="O31" s="19"/>
+      <c r="P31" s="19"/>
+      <c r="Q31" s="19"/>
+      <c r="R31" s="19"/>
+      <c r="S31" s="19"/>
+      <c r="T31" s="19"/>
+      <c r="U31" s="19"/>
+      <c r="V31" s="19"/>
+      <c r="W31" s="19"/>
+      <c r="X31" s="19"/>
+      <c r="Y31" s="19"/>
+      <c r="Z31" s="19"/>
+      <c r="AA31" s="19"/>
     </row>
     <row r="32" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A32" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="B32" s="17" t="s">
-        <v>50</v>
+      <c r="A32" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>26</v>
       </c>
       <c r="C32" s="10"/>
-      <c r="D32" s="15" t="s">
-        <v>47</v>
+      <c r="D32" s="14" t="s">
+        <v>24</v>
       </c>
       <c r="E32" s="6"/>
       <c r="F32" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="G32" s="20"/>
-      <c r="H32" s="20"/>
-      <c r="I32" s="20"/>
-      <c r="J32" s="20"/>
-      <c r="K32" s="20"/>
-      <c r="L32" s="20"/>
-      <c r="M32" s="20"/>
-      <c r="N32" s="20"/>
-      <c r="O32" s="20"/>
-      <c r="P32" s="20"/>
-      <c r="Q32" s="20"/>
-      <c r="R32" s="20"/>
-      <c r="S32" s="20"/>
-      <c r="T32" s="20"/>
-      <c r="U32" s="20"/>
-      <c r="V32" s="20"/>
-      <c r="W32" s="20"/>
-      <c r="X32" s="20"/>
-      <c r="Y32" s="20"/>
-      <c r="Z32" s="20"/>
-      <c r="AA32" s="20"/>
+        <v>39</v>
+      </c>
+      <c r="G32" s="19"/>
+      <c r="H32" s="19"/>
+      <c r="I32" s="19"/>
+      <c r="J32" s="19"/>
+      <c r="K32" s="19"/>
+      <c r="L32" s="19"/>
+      <c r="M32" s="19"/>
+      <c r="N32" s="19"/>
+      <c r="O32" s="19"/>
+      <c r="P32" s="19"/>
+      <c r="Q32" s="19"/>
+      <c r="R32" s="19"/>
+      <c r="S32" s="19"/>
+      <c r="T32" s="19"/>
+      <c r="U32" s="19"/>
+      <c r="V32" s="19"/>
+      <c r="W32" s="19"/>
+      <c r="X32" s="19"/>
+      <c r="Y32" s="19"/>
+      <c r="Z32" s="19"/>
+      <c r="AA32" s="19"/>
     </row>
     <row r="33" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A33" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="B33" s="15" t="s">
-        <v>52</v>
+      <c r="A33" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>27</v>
       </c>
       <c r="C33" s="10"/>
-      <c r="D33" s="15" t="s">
-        <v>19</v>
+      <c r="D33" s="14" t="s">
+        <v>12</v>
       </c>
       <c r="E33" s="6"/>
       <c r="F33" s="10" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A34" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="B34" s="15" t="s">
-        <v>53</v>
+      <c r="A34" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>28</v>
       </c>
       <c r="C34" s="10"/>
-      <c r="D34" s="15" t="s">
-        <v>88</v>
+      <c r="D34" s="14" t="s">
+        <v>54</v>
       </c>
       <c r="E34" s="6"/>
       <c r="F34" s="10" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A35" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="B35" s="15" t="s">
-        <v>53</v>
+      <c r="A35" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>28</v>
       </c>
       <c r="C35" s="10"/>
-      <c r="D35" s="15" t="s">
-        <v>88</v>
+      <c r="D35" s="14" t="s">
+        <v>54</v>
       </c>
       <c r="E35" s="6"/>
       <c r="F35" s="10" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A36" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="B36" s="15" t="s">
-        <v>53</v>
+      <c r="A36" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>28</v>
       </c>
       <c r="C36" s="10"/>
-      <c r="D36" s="15" t="s">
-        <v>88</v>
+      <c r="D36" s="14" t="s">
+        <v>54</v>
       </c>
       <c r="E36" s="6"/>
       <c r="F36" s="10" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A37" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="B37" s="15" t="s">
-        <v>53</v>
+      <c r="A37" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>28</v>
       </c>
       <c r="C37" s="10"/>
-      <c r="D37" s="15" t="s">
-        <v>88</v>
+      <c r="D37" s="14" t="s">
+        <v>54</v>
       </c>
       <c r="E37" s="6"/>
       <c r="F37" s="10" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A38" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="B38" s="15" t="s">
-        <v>53</v>
+      <c r="A38" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>28</v>
       </c>
       <c r="C38" s="10"/>
-      <c r="D38" s="15" t="s">
-        <v>88</v>
+      <c r="D38" s="14" t="s">
+        <v>54</v>
       </c>
       <c r="E38" s="6"/>
       <c r="F38" s="10" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A39" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="B39" s="15" t="s">
-        <v>53</v>
+      <c r="A39" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="B39" s="14" t="s">
+        <v>28</v>
       </c>
       <c r="C39" s="10"/>
-      <c r="D39" s="15" t="s">
-        <v>88</v>
+      <c r="D39" s="14" t="s">
+        <v>54</v>
       </c>
       <c r="E39" s="6"/>
       <c r="F39" s="10" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A40" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="B40" s="15" t="s">
-        <v>53</v>
+      <c r="A40" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="B40" s="14" t="s">
+        <v>28</v>
       </c>
       <c r="C40" s="10"/>
-      <c r="D40" s="15" t="s">
-        <v>88</v>
+      <c r="D40" s="14" t="s">
+        <v>54</v>
       </c>
       <c r="E40" s="6"/>
       <c r="F40" s="10" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A41" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="B41" s="15" t="s">
-        <v>53</v>
+      <c r="A41" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="B41" s="14" t="s">
+        <v>28</v>
       </c>
       <c r="C41" s="10"/>
-      <c r="D41" s="15" t="s">
-        <v>88</v>
+      <c r="D41" s="14" t="s">
+        <v>54</v>
       </c>
       <c r="E41" s="6"/>
       <c r="F41" s="10" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A42" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="B42" s="21" t="s">
-        <v>53</v>
+      <c r="A42" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="B42" s="20" t="s">
+        <v>28</v>
       </c>
       <c r="C42" s="10"/>
-      <c r="D42" s="21" t="s">
-        <v>88</v>
+      <c r="D42" s="20" t="s">
+        <v>54</v>
       </c>
       <c r="E42" s="6"/>
       <c r="F42" s="10" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A43" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="B43" s="21" t="s">
-        <v>53</v>
+      <c r="A43" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="B43" s="20" t="s">
+        <v>28</v>
       </c>
       <c r="C43" s="10"/>
-      <c r="D43" s="21" t="s">
-        <v>88</v>
+      <c r="D43" s="20" t="s">
+        <v>54</v>
       </c>
       <c r="E43" s="6"/>
       <c r="F43" s="10" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A44" s="21" t="s">
-        <v>98</v>
-      </c>
-      <c r="B44" s="21" t="s">
-        <v>53</v>
+      <c r="A44" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="B44" s="20" t="s">
+        <v>28</v>
       </c>
       <c r="C44" s="10"/>
-      <c r="D44" s="21" t="s">
-        <v>88</v>
+      <c r="D44" s="20" t="s">
+        <v>54</v>
       </c>
       <c r="E44" s="6"/>
       <c r="F44" s="10" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A45" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="B45" s="21" t="s">
-        <v>53</v>
+      <c r="A45" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="B45" s="20" t="s">
+        <v>28</v>
       </c>
       <c r="C45" s="10"/>
-      <c r="D45" s="21" t="s">
-        <v>88</v>
+      <c r="D45" s="20" t="s">
+        <v>54</v>
       </c>
       <c r="E45" s="6"/>
       <c r="F45" s="10" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A46" s="21" t="s">
-        <v>100</v>
-      </c>
-      <c r="B46" s="21" t="s">
-        <v>53</v>
+      <c r="A46" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="B46" s="20" t="s">
+        <v>28</v>
       </c>
       <c r="C46" s="10"/>
-      <c r="D46" s="21" t="s">
-        <v>88</v>
+      <c r="D46" s="20" t="s">
+        <v>54</v>
       </c>
       <c r="E46" s="6"/>
       <c r="F46" s="10" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A47" s="21" t="s">
-        <v>101</v>
-      </c>
-      <c r="B47" s="21" t="s">
-        <v>53</v>
+      <c r="A47" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="B47" s="20" t="s">
+        <v>28</v>
       </c>
       <c r="C47" s="10"/>
-      <c r="D47" s="21" t="s">
-        <v>88</v>
+      <c r="D47" s="20" t="s">
+        <v>54</v>
       </c>
       <c r="E47" s="6"/>
       <c r="F47" s="10" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A48" s="21" t="s">
-        <v>102</v>
-      </c>
-      <c r="B48" s="21" t="s">
-        <v>53</v>
+      <c r="A48" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="B48" s="20" t="s">
+        <v>28</v>
       </c>
       <c r="C48" s="10"/>
-      <c r="D48" s="21" t="s">
-        <v>88</v>
+      <c r="D48" s="20" t="s">
+        <v>54</v>
       </c>
       <c r="E48" s="6"/>
       <c r="F48" s="10" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A49" s="21" t="s">
-        <v>103</v>
-      </c>
-      <c r="B49" s="21" t="s">
-        <v>53</v>
+      <c r="A49" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="B49" s="20" t="s">
+        <v>28</v>
       </c>
       <c r="C49" s="10"/>
-      <c r="D49" s="21" t="s">
-        <v>88</v>
+      <c r="D49" s="20" t="s">
+        <v>54</v>
       </c>
       <c r="E49" s="6"/>
       <c r="F49" s="10" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A50" s="21" t="s">
-        <v>104</v>
-      </c>
-      <c r="B50" s="21" t="s">
-        <v>53</v>
+      <c r="A50" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="B50" s="20" t="s">
+        <v>28</v>
       </c>
       <c r="C50" s="10"/>
-      <c r="D50" s="21" t="s">
-        <v>88</v>
+      <c r="D50" s="20" t="s">
+        <v>54</v>
       </c>
       <c r="E50" s="6"/>
       <c r="F50" s="10" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A51" s="21" t="s">
-        <v>105</v>
-      </c>
-      <c r="B51" s="21" t="s">
-        <v>53</v>
+      <c r="A51" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="B51" s="20" t="s">
+        <v>28</v>
       </c>
       <c r="C51" s="10"/>
-      <c r="D51" s="21" t="s">
-        <v>88</v>
+      <c r="D51" s="20" t="s">
+        <v>54</v>
       </c>
       <c r="E51" s="6"/>
       <c r="F51" s="10" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A52" s="21" t="s">
-        <v>106</v>
-      </c>
-      <c r="B52" s="21" t="s">
-        <v>53</v>
+      <c r="A52" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="B52" s="20" t="s">
+        <v>28</v>
       </c>
       <c r="C52" s="10"/>
-      <c r="D52" s="21" t="s">
-        <v>88</v>
+      <c r="D52" s="20" t="s">
+        <v>54</v>
       </c>
       <c r="E52" s="6"/>
       <c r="F52" s="10" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>107</v>
+      <c r="A53" s="25" t="s">
+        <v>113</v>
       </c>
       <c r="B53" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="C53" s="6"/>
       <c r="D53" t="s">
-        <v>88</v>
+        <v>54</v>
       </c>
       <c r="E53" s="6"/>
       <c r="F53" s="10" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>108</v>
+      <c r="A54" s="25" t="s">
+        <v>114</v>
       </c>
       <c r="B54" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="C54" s="6"/>
       <c r="D54" t="s">
-        <v>88</v>
+        <v>54</v>
       </c>
       <c r="E54" s="6"/>
       <c r="F54" s="10" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>109</v>
+      <c r="A55" s="25" t="s">
+        <v>115</v>
       </c>
       <c r="B55" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="C55" s="6"/>
       <c r="D55" t="s">
-        <v>88</v>
+        <v>54</v>
       </c>
       <c r="E55" s="6"/>
       <c r="F55" s="10" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>55</v>
+      <c r="A56" s="25" t="s">
+        <v>116</v>
       </c>
       <c r="B56" t="s">
-        <v>113</v>
+        <v>57</v>
       </c>
       <c r="C56" s="6"/>
       <c r="D56" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E56" s="6"/>
       <c r="F56" s="10" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>56</v>
+      <c r="A57" s="25" t="s">
+        <v>117</v>
       </c>
       <c r="B57" t="s">
-        <v>57</v>
-      </c>
-      <c r="C57" s="6"/>
+        <v>61</v>
+      </c>
+      <c r="C57" s="10"/>
       <c r="D57" t="s">
+        <v>62</v>
+      </c>
+      <c r="E57" s="10"/>
+      <c r="F57" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A58" s="25" t="s">
         <v>118</v>
       </c>
-      <c r="E57" s="6"/>
-      <c r="F57" s="10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>59</v>
-      </c>
       <c r="B58" t="s">
-        <v>60</v>
-      </c>
-      <c r="C58" s="6"/>
+        <v>63</v>
+      </c>
+      <c r="C58" s="10"/>
       <c r="D58" t="s">
-        <v>118</v>
-      </c>
-      <c r="E58" s="6"/>
+        <v>62</v>
+      </c>
+      <c r="E58" s="10"/>
       <c r="F58" s="10" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>61</v>
+      <c r="A59" s="25" t="s">
+        <v>119</v>
       </c>
       <c r="B59" t="s">
+        <v>64</v>
+      </c>
+      <c r="C59" s="10"/>
+      <c r="D59" t="s">
         <v>62</v>
       </c>
-      <c r="C59" s="6"/>
-      <c r="D59" t="s">
-        <v>118</v>
-      </c>
-      <c r="E59" s="6"/>
+      <c r="E59" s="10"/>
       <c r="F59" s="10" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>114</v>
+      <c r="A60" s="25" t="s">
+        <v>120</v>
       </c>
       <c r="B60" t="s">
-        <v>63</v>
-      </c>
-      <c r="C60" s="6"/>
+        <v>65</v>
+      </c>
+      <c r="C60" s="10"/>
       <c r="D60" t="s">
-        <v>47</v>
-      </c>
-      <c r="E60" s="6"/>
+        <v>62</v>
+      </c>
+      <c r="E60" s="10"/>
       <c r="F60" s="10" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>115</v>
+      <c r="A61" s="25" t="s">
+        <v>121</v>
       </c>
       <c r="B61" t="s">
-        <v>64</v>
+        <v>30</v>
       </c>
       <c r="C61" s="6"/>
       <c r="D61" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="E61" s="6"/>
       <c r="F61" s="10" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>116</v>
+      <c r="A62" s="25" t="s">
+        <v>122</v>
       </c>
       <c r="B62" t="s">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="C62" s="6"/>
       <c r="D62" t="s">
-        <v>58</v>
+        <v>12</v>
       </c>
       <c r="E62" s="6"/>
       <c r="F62" s="10" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>117</v>
+      <c r="A63" s="25" t="s">
+        <v>123</v>
       </c>
       <c r="B63" t="s">
-        <v>66</v>
+        <v>33</v>
       </c>
       <c r="C63" s="6"/>
       <c r="D63" t="s">
-        <v>58</v>
+        <v>12</v>
       </c>
       <c r="E63" s="6"/>
       <c r="F63" s="10" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>69</v>
+      <c r="A64" s="25" t="s">
+        <v>124</v>
       </c>
       <c r="B64" t="s">
-        <v>70</v>
+        <v>34</v>
       </c>
       <c r="C64" s="6"/>
       <c r="D64" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="E64" s="6"/>
       <c r="F64" s="10" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>71</v>
+      <c r="A65" s="25" t="s">
+        <v>125</v>
       </c>
       <c r="B65" t="s">
-        <v>72</v>
+        <v>35</v>
       </c>
       <c r="C65" s="6"/>
       <c r="D65" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="E65" s="6"/>
       <c r="F65" s="10" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>73</v>
+      <c r="A66" s="25" t="s">
+        <v>126</v>
       </c>
       <c r="B66" t="s">
-        <v>74</v>
+        <v>36</v>
       </c>
       <c r="C66" s="6"/>
       <c r="D66" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
       <c r="E66" s="6"/>
       <c r="F66" s="10" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A67" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="B67" t="s">
+        <v>37</v>
+      </c>
       <c r="C67" s="6"/>
+      <c r="D67" t="s">
+        <v>31</v>
+      </c>
       <c r="E67" s="6"/>
-      <c r="F67" s="6"/>
+      <c r="F67" s="10" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="68" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A68" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="B68" t="s">
+        <v>40</v>
+      </c>
       <c r="C68" s="6"/>
+      <c r="D68" t="s">
+        <v>9</v>
+      </c>
       <c r="E68" s="6"/>
-      <c r="F68" s="6"/>
+      <c r="F68" s="10" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="69" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A69" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="B69" t="s">
+        <v>41</v>
+      </c>
       <c r="C69" s="6"/>
+      <c r="D69" t="s">
+        <v>29</v>
+      </c>
       <c r="E69" s="6"/>
-      <c r="F69" s="6"/>
+      <c r="F69" s="10" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="70" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A70" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="B70" t="s">
+        <v>42</v>
+      </c>
       <c r="C70" s="6"/>
+      <c r="D70" t="s">
+        <v>29</v>
+      </c>
       <c r="E70" s="6"/>
-      <c r="F70" s="6"/>
+      <c r="F70" s="10" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="71" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C71" s="6"/>
@@ -6678,99 +6856,134 @@
       <c r="F1003" s="6"/>
     </row>
     <row r="1004" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="E1004" s="22"/>
-      <c r="F1004" s="22"/>
+      <c r="C1004" s="6"/>
+      <c r="E1004" s="6"/>
+      <c r="F1004" s="6"/>
     </row>
     <row r="1005" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="E1005" s="22"/>
-      <c r="F1005" s="22"/>
+      <c r="C1005" s="6"/>
+      <c r="E1005" s="6"/>
+      <c r="F1005" s="6"/>
     </row>
     <row r="1006" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="E1006" s="22"/>
-      <c r="F1006" s="22"/>
+      <c r="C1006" s="6"/>
+      <c r="E1006" s="6"/>
+      <c r="F1006" s="6"/>
     </row>
     <row r="1007" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="E1007" s="22"/>
-      <c r="F1007" s="22"/>
+      <c r="C1007" s="6"/>
+      <c r="E1007" s="6"/>
+      <c r="F1007" s="6"/>
     </row>
     <row r="1008" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="E1008" s="22"/>
-      <c r="F1008" s="22"/>
+      <c r="E1008" s="21"/>
+      <c r="F1008" s="21"/>
     </row>
     <row r="1009" spans="5:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="E1009" s="22"/>
-      <c r="F1009" s="22"/>
+      <c r="E1009" s="21"/>
+      <c r="F1009" s="21"/>
     </row>
     <row r="1010" spans="5:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="E1010" s="22"/>
-      <c r="F1010" s="22"/>
+      <c r="E1010" s="21"/>
+      <c r="F1010" s="21"/>
     </row>
     <row r="1011" spans="5:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="E1011" s="22"/>
-      <c r="F1011" s="22"/>
+      <c r="E1011" s="21"/>
+      <c r="F1011" s="21"/>
     </row>
     <row r="1012" spans="5:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="E1012" s="22"/>
-      <c r="F1012" s="22"/>
+      <c r="E1012" s="21"/>
+      <c r="F1012" s="21"/>
     </row>
     <row r="1013" spans="5:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="E1013" s="22"/>
-      <c r="F1013" s="22"/>
+      <c r="E1013" s="21"/>
+      <c r="F1013" s="21"/>
     </row>
     <row r="1014" spans="5:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="E1014" s="22"/>
-      <c r="F1014" s="22"/>
+      <c r="E1014" s="21"/>
+      <c r="F1014" s="21"/>
     </row>
     <row r="1015" spans="5:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="E1015" s="22"/>
-      <c r="F1015" s="22"/>
+      <c r="E1015" s="21"/>
+      <c r="F1015" s="21"/>
     </row>
     <row r="1016" spans="5:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="E1016" s="22"/>
-      <c r="F1016" s="22"/>
+      <c r="E1016" s="21"/>
+      <c r="F1016" s="21"/>
     </row>
     <row r="1017" spans="5:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="E1017" s="22"/>
-      <c r="F1017" s="22"/>
+      <c r="E1017" s="21"/>
+      <c r="F1017" s="21"/>
     </row>
     <row r="1018" spans="5:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="E1018" s="22"/>
-      <c r="F1018" s="22"/>
+      <c r="E1018" s="21"/>
+      <c r="F1018" s="21"/>
     </row>
     <row r="1019" spans="5:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="E1019" s="22"/>
-      <c r="F1019" s="22"/>
+      <c r="E1019" s="21"/>
+      <c r="F1019" s="21"/>
     </row>
     <row r="1020" spans="5:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="E1020" s="22"/>
-      <c r="F1020" s="22"/>
+      <c r="E1020" s="21"/>
+      <c r="F1020" s="21"/>
+    </row>
+    <row r="1021" spans="5:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="E1021" s="21"/>
+      <c r="F1021" s="21"/>
+    </row>
+    <row r="1022" spans="5:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="E1022" s="21"/>
+      <c r="F1022" s="21"/>
+    </row>
+    <row r="1023" spans="5:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="E1023" s="21"/>
+      <c r="F1023" s="21"/>
+    </row>
+    <row r="1024" spans="5:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="E1024" s="21"/>
+      <c r="F1024" s="21"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F2:F1020">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+  <conditionalFormatting sqref="F2:F1024">
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
       <formula>"Developed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:F1020">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+  <conditionalFormatting sqref="E2:F56 E61:F1024 F57:F60">
+    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E1020">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+  <conditionalFormatting sqref="E2:E56 E61:E1024">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>"Tested"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E1020">
-    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
+  <conditionalFormatting sqref="E2:E56 E61:E1024">
+    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
+      <formula>"Issue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E57:E60">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+      <formula>"Pending"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E57:E60">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>"Tested"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E57:E60">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"Issue"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" sqref="F2:F1020">
+    <dataValidation type="list" allowBlank="1" sqref="F2:F1024">
       <formula1>"Developed,Pending"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="E2:E1020">
+    <dataValidation type="list" allowBlank="1" sqref="E2:E1024">
       <formula1>"Tested,Pending,Issue"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
expoPalletSearch, expoPalletDelete, expoPalletDeleteAllRecords, expoPalletImportExcel, exportImportExcel
</commit_message>
<xml_diff>
--- a/tests/TestCasesPlan.xlsx
+++ b/tests/TestCasesPlan.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="133">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Amna</t>
   </si>
   <si>
-    <t>Test SKU management in Expoloader ImportExel</t>
-  </si>
-  <si>
     <t>Test SKU management in Expoloader edit</t>
   </si>
   <si>
@@ -418,6 +415,9 @@
   </si>
   <si>
     <t>navExpoloader</t>
+  </si>
+  <si>
+    <t>Test SKU management in Expoloader exportExel</t>
   </si>
 </sst>
 </file>
@@ -586,23 +586,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF9900"/>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF6AA84F"/>
-          <bgColor rgb="FF6AA84F"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="7">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -624,46 +608,6 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFFF9900"/>
           <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF6AA84F"/>
-          <bgColor rgb="FF6AA84F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCC0000"/>
-          <bgColor rgb="FFCC0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF6AA84F"/>
-          <bgColor rgb="FF6AA84F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF9900"/>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF6AA84F"/>
-          <bgColor rgb="FF6AA84F"/>
         </patternFill>
       </fill>
     </dxf>
@@ -915,8 +859,8 @@
   </sheetPr>
   <dimension ref="A1:AA1024"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -950,25 +894,25 @@
     </row>
     <row r="2" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="22" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E2" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>38</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A3" s="22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>7</v>
@@ -979,15 +923,15 @@
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A4" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="13" t="s">
@@ -995,15 +939,15 @@
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A5" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="14" t="s">
@@ -1011,15 +955,15 @@
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A6" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>10</v>
+        <v>132</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="14" t="s">
@@ -1027,15 +971,15 @@
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A7" s="26" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="14" t="s">
@@ -1043,313 +987,323 @@
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A8" s="26" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E8" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="10" t="s">
         <v>38</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A9" s="26" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E9" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="10" t="s">
         <v>38</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A10" s="26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E10" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="10" t="s">
         <v>38</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A11" s="26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="6"/>
+        <v>11</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="F11" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A12" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A13" s="22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A14" s="26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14" s="10"/>
       <c r="D14" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A15" s="26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E15" s="6"/>
       <c r="F15" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A16" s="26" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E16" s="6"/>
       <c r="F16" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:27" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A17" s="22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C17" s="10"/>
       <c r="D17" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E17" s="6"/>
       <c r="F17" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A18" s="22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E18" s="10"/>
       <c r="F18" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A19" s="22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C19" s="10"/>
       <c r="D19" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E19" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F19" s="10" t="s">
         <v>38</v>
-      </c>
-      <c r="F19" s="10" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A20" s="22" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C20" s="10"/>
       <c r="D20" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" s="6"/>
+        <v>11</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="F20" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A21" s="26" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C21" s="10"/>
       <c r="D21" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E21" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F21" s="10" t="s">
         <v>38</v>
-      </c>
-      <c r="F21" s="10" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A22" s="26" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C22" s="10"/>
       <c r="D22" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="E22" s="6"/>
+        <v>11</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="F22" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A23" s="26" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C23" s="10"/>
       <c r="D23" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="E23" s="6"/>
+        <v>11</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="F23" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:27" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A24" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C24" s="10"/>
       <c r="D24" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24" s="6"/>
+        <v>11</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="F24" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A25" s="22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C25" s="10"/>
       <c r="D25" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E25" s="10"/>
       <c r="F25" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:27" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A26" s="22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C26" s="10"/>
       <c r="D26" s="13" t="s">
@@ -1357,15 +1311,15 @@
       </c>
       <c r="E26" s="6"/>
       <c r="F26" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:27" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A27" s="22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C27" s="10"/>
       <c r="D27" s="18" t="s">
@@ -1373,7 +1327,7 @@
       </c>
       <c r="E27" s="6"/>
       <c r="F27" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G27" s="19"/>
       <c r="H27" s="19"/>
@@ -1399,18 +1353,18 @@
     </row>
     <row r="28" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A28" s="22" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C28" s="10"/>
       <c r="D28" s="24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E28" s="10"/>
       <c r="F28" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G28" s="19"/>
       <c r="H28" s="19"/>
@@ -1436,18 +1390,18 @@
     </row>
     <row r="29" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A29" s="22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C29" s="10"/>
       <c r="D29" s="13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E29" s="6"/>
       <c r="F29" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G29" s="19"/>
       <c r="H29" s="19"/>
@@ -1473,18 +1427,18 @@
     </row>
     <row r="30" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A30" s="22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C30" s="10"/>
       <c r="D30" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E30" s="6"/>
       <c r="F30" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G30" s="19"/>
       <c r="H30" s="19"/>
@@ -1510,18 +1464,18 @@
     </row>
     <row r="31" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A31" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C31" s="10"/>
       <c r="D31" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E31" s="6"/>
       <c r="F31" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G31" s="19"/>
       <c r="H31" s="19"/>
@@ -1547,18 +1501,18 @@
     </row>
     <row r="32" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A32" s="22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C32" s="10"/>
       <c r="D32" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E32" s="6"/>
       <c r="F32" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G32" s="19"/>
       <c r="H32" s="19"/>
@@ -1584,378 +1538,378 @@
     </row>
     <row r="33" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A33" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B33" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C33" s="10"/>
       <c r="D33" s="14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E33" s="6"/>
       <c r="F33" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A34" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C34" s="10"/>
       <c r="D34" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E34" s="6"/>
       <c r="F34" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A35" s="27" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B35" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C35" s="10"/>
       <c r="D35" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E35" s="6"/>
       <c r="F35" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A36" s="27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B36" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C36" s="10"/>
       <c r="D36" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E36" s="6"/>
       <c r="F36" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A37" s="27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B37" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C37" s="10"/>
       <c r="D37" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E37" s="6"/>
       <c r="F37" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A38" s="27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C38" s="10"/>
       <c r="D38" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E38" s="6"/>
       <c r="F38" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A39" s="27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B39" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C39" s="10"/>
       <c r="D39" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E39" s="6"/>
       <c r="F39" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A40" s="27" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B40" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C40" s="10"/>
       <c r="D40" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E40" s="6"/>
       <c r="F40" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A41" s="27" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B41" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C41" s="10"/>
       <c r="D41" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E41" s="6"/>
       <c r="F41" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="28" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B42" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C42" s="10"/>
       <c r="D42" s="20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E42" s="6"/>
       <c r="F42" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="28" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B43" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C43" s="10"/>
       <c r="D43" s="20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E43" s="6"/>
       <c r="F43" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="28" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B44" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C44" s="10"/>
       <c r="D44" s="20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E44" s="6"/>
       <c r="F44" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="28" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B45" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C45" s="10"/>
       <c r="D45" s="20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E45" s="6"/>
       <c r="F45" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B46" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C46" s="10"/>
       <c r="D46" s="20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E46" s="6"/>
       <c r="F46" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="28" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B47" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C47" s="10"/>
       <c r="D47" s="20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E47" s="6"/>
       <c r="F47" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="28" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B48" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C48" s="10"/>
       <c r="D48" s="20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E48" s="6"/>
       <c r="F48" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="28" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B49" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C49" s="10"/>
       <c r="D49" s="20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E49" s="6"/>
       <c r="F49" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="28" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B50" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C50" s="10"/>
       <c r="D50" s="20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E50" s="6"/>
       <c r="F50" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="28" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B51" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C51" s="10"/>
       <c r="D51" s="20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E51" s="6"/>
       <c r="F51" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="28" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B52" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C52" s="10"/>
       <c r="D52" s="20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E52" s="6"/>
       <c r="F52" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="25" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B53" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C53" s="6"/>
       <c r="D53" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E53" s="6"/>
       <c r="F53" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="25" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B54" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C54" s="6"/>
       <c r="D54" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E54" s="6"/>
       <c r="F54" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="25" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B55" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C55" s="6"/>
       <c r="D55" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E55" s="6"/>
       <c r="F55" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="25" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B56" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C56" s="6"/>
       <c r="D56" t="s">
@@ -1963,191 +1917,191 @@
       </c>
       <c r="E56" s="6"/>
       <c r="F56" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="25" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B57" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C57" s="10"/>
       <c r="D57" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E57" s="10"/>
       <c r="F57" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="25" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B58" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C58" s="10"/>
       <c r="D58" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E58" s="10"/>
       <c r="F58" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="25" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B59" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C59" s="10"/>
       <c r="D59" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E59" s="10"/>
       <c r="F59" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B60" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C60" s="10"/>
       <c r="D60" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E60" s="10"/>
       <c r="F60" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="25" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B61" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C61" s="6"/>
       <c r="D61" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E61" s="6"/>
       <c r="F61" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="25" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B62" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C62" s="6"/>
       <c r="D62" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E62" s="6"/>
       <c r="F62" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" s="25" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B63" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C63" s="6"/>
       <c r="D63" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E63" s="6"/>
       <c r="F63" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A64" s="25" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B64" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C64" s="6"/>
       <c r="D64" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E64" s="6"/>
       <c r="F64" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A65" s="25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B65" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C65" s="6"/>
       <c r="D65" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E65" s="6"/>
       <c r="F65" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A66" s="25" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B66" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C66" s="6"/>
       <c r="D66" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E66" s="6"/>
       <c r="F66" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A67" s="25" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B67" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C67" s="6"/>
       <c r="D67" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E67" s="6"/>
       <c r="F67" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A68" s="25" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B68" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C68" s="6"/>
       <c r="D68" t="s">
@@ -2155,39 +2109,39 @@
       </c>
       <c r="E68" s="6"/>
       <c r="F68" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A69" s="25" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B69" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C69" s="6"/>
       <c r="D69" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E69" s="6"/>
       <c r="F69" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A70" s="25" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B70" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C70" s="6"/>
       <c r="D70" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E70" s="6"/>
       <c r="F70" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -6945,37 +6899,37 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F2:F1024">
-    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
       <formula>"Developed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:F56 E61:F1024 F57:F60">
-    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E56 E61:E1024">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
       <formula>"Tested"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E56 E61:E1024">
-    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="9" operator="equal">
       <formula>"Issue"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E57:E60">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E57:E60">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"Tested"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E57:E60">
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>"Issue"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Updated test cases plan and added new issue in Issues ILT
</commit_message>
<xml_diff>
--- a/tests/TestCasesPlan.xlsx
+++ b/tests/TestCasesPlan.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="136">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -198,9 +198,6 @@
     <t>SKU import excel data</t>
   </si>
   <si>
-    <t>container export excel data</t>
-  </si>
-  <si>
     <t>test project add</t>
   </si>
   <si>
@@ -418,6 +415,18 @@
   </si>
   <si>
     <t>Test SKU management in Expoloader exportExel</t>
+  </si>
+  <si>
+    <t>pallet export excel data</t>
+  </si>
+  <si>
+    <t>forgetPassword</t>
+  </si>
+  <si>
+    <t>test forget password</t>
+  </si>
+  <si>
+    <t>Pending</t>
   </si>
 </sst>
 </file>
@@ -859,8 +868,8 @@
   </sheetPr>
   <dimension ref="A1:AA1024"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -894,7 +903,7 @@
     </row>
     <row r="2" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>6</v>
@@ -912,7 +921,7 @@
     </row>
     <row r="3" spans="1:6" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A3" s="22" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>7</v>
@@ -928,7 +937,7 @@
     </row>
     <row r="4" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A4" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>54</v>
@@ -944,7 +953,7 @@
     </row>
     <row r="5" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A5" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>42</v>
@@ -960,10 +969,10 @@
     </row>
     <row r="6" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A6" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="14" t="s">
@@ -976,7 +985,7 @@
     </row>
     <row r="7" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A7" s="26" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>10</v>
@@ -992,7 +1001,7 @@
     </row>
     <row r="8" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A8" s="26" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>43</v>
@@ -1010,7 +1019,7 @@
     </row>
     <row r="9" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A9" s="26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>44</v>
@@ -1028,7 +1037,7 @@
     </row>
     <row r="10" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A10" s="26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>45</v>
@@ -1046,7 +1055,7 @@
     </row>
     <row r="11" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A11" s="26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>58</v>
@@ -1064,7 +1073,7 @@
     </row>
     <row r="12" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A12" s="22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>12</v>
@@ -1080,7 +1089,7 @@
     </row>
     <row r="13" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A13" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>14</v>
@@ -1096,7 +1105,7 @@
     </row>
     <row r="14" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A14" s="26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>16</v>
@@ -1112,7 +1121,7 @@
     </row>
     <row r="15" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A15" s="26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>46</v>
@@ -1128,7 +1137,7 @@
     </row>
     <row r="16" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A16" s="26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>47</v>
@@ -1144,7 +1153,7 @@
     </row>
     <row r="17" spans="1:27" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A17" s="22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>48</v>
@@ -1160,7 +1169,7 @@
     </row>
     <row r="18" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A18" s="22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>57</v>
@@ -1169,14 +1178,16 @@
       <c r="D18" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E18" s="10"/>
+      <c r="E18" s="10" t="s">
+        <v>37</v>
+      </c>
       <c r="F18" s="10" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A19" s="22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B19" s="9" t="s">
         <v>49</v>
@@ -1194,7 +1205,7 @@
     </row>
     <row r="20" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A20" s="22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>18</v>
@@ -1212,7 +1223,7 @@
     </row>
     <row r="21" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A21" s="26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>19</v>
@@ -1230,7 +1241,7 @@
     </row>
     <row r="22" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A22" s="26" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B22" s="9" t="s">
         <v>50</v>
@@ -1248,7 +1259,7 @@
     </row>
     <row r="23" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A23" s="26" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B23" s="9" t="s">
         <v>51</v>
@@ -1266,7 +1277,7 @@
     </row>
     <row r="24" spans="1:27" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A24" s="22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B24" s="9" t="s">
         <v>52</v>
@@ -1284,23 +1295,25 @@
     </row>
     <row r="25" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A25" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>59</v>
+        <v>132</v>
       </c>
       <c r="C25" s="10"/>
       <c r="D25" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E25" s="10"/>
+      <c r="E25" s="10" t="s">
+        <v>37</v>
+      </c>
       <c r="F25" s="10" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:27" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A26" s="22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B26" s="9" t="s">
         <v>20</v>
@@ -1316,7 +1329,7 @@
     </row>
     <row r="27" spans="1:27" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A27" s="22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B27" s="17" t="s">
         <v>20</v>
@@ -1353,7 +1366,7 @@
     </row>
     <row r="28" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A28" s="22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B28" s="23" t="s">
         <v>55</v>
@@ -1390,7 +1403,7 @@
     </row>
     <row r="29" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A29" s="22" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B29" s="18" t="s">
         <v>21</v>
@@ -1399,7 +1412,9 @@
       <c r="D29" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E29" s="6"/>
+      <c r="E29" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="F29" s="10" t="s">
         <v>38</v>
       </c>
@@ -1501,7 +1516,7 @@
     </row>
     <row r="32" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A32" s="22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B32" s="16" t="s">
         <v>25</v>
@@ -1538,7 +1553,7 @@
     </row>
     <row r="33" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A33" s="27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B33" s="14" t="s">
         <v>26</v>
@@ -1547,14 +1562,16 @@
       <c r="D33" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E33" s="6"/>
+      <c r="E33" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="F33" s="10" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A34" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B34" s="14" t="s">
         <v>27</v>
@@ -1570,7 +1587,7 @@
     </row>
     <row r="35" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A35" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B35" s="14" t="s">
         <v>27</v>
@@ -1586,7 +1603,7 @@
     </row>
     <row r="36" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A36" s="27" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B36" s="14" t="s">
         <v>27</v>
@@ -1602,7 +1619,7 @@
     </row>
     <row r="37" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A37" s="27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B37" s="14" t="s">
         <v>27</v>
@@ -1618,7 +1635,7 @@
     </row>
     <row r="38" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A38" s="27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B38" s="14" t="s">
         <v>27</v>
@@ -1634,7 +1651,7 @@
     </row>
     <row r="39" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A39" s="27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B39" s="14" t="s">
         <v>27</v>
@@ -1650,7 +1667,7 @@
     </row>
     <row r="40" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A40" s="27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B40" s="14" t="s">
         <v>27</v>
@@ -1666,7 +1683,7 @@
     </row>
     <row r="41" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A41" s="27" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B41" s="14" t="s">
         <v>27</v>
@@ -1682,7 +1699,7 @@
     </row>
     <row r="42" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="28" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B42" s="20" t="s">
         <v>27</v>
@@ -1698,7 +1715,7 @@
     </row>
     <row r="43" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="28" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B43" s="20" t="s">
         <v>27</v>
@@ -1714,7 +1731,7 @@
     </row>
     <row r="44" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="28" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B44" s="20" t="s">
         <v>27</v>
@@ -1730,7 +1747,7 @@
     </row>
     <row r="45" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="28" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B45" s="20" t="s">
         <v>27</v>
@@ -1746,7 +1763,7 @@
     </row>
     <row r="46" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="28" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B46" s="20" t="s">
         <v>27</v>
@@ -1762,7 +1779,7 @@
     </row>
     <row r="47" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B47" s="20" t="s">
         <v>27</v>
@@ -1778,7 +1795,7 @@
     </row>
     <row r="48" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="28" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B48" s="20" t="s">
         <v>27</v>
@@ -1794,7 +1811,7 @@
     </row>
     <row r="49" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="28" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B49" s="20" t="s">
         <v>27</v>
@@ -1810,7 +1827,7 @@
     </row>
     <row r="50" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="28" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B50" s="20" t="s">
         <v>27</v>
@@ -1826,7 +1843,7 @@
     </row>
     <row r="51" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="28" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B51" s="20" t="s">
         <v>27</v>
@@ -1842,7 +1859,7 @@
     </row>
     <row r="52" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="28" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B52" s="20" t="s">
         <v>27</v>
@@ -1858,7 +1875,7 @@
     </row>
     <row r="53" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="25" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B53" t="s">
         <v>27</v>
@@ -1874,7 +1891,7 @@
     </row>
     <row r="54" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="25" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B54" t="s">
         <v>27</v>
@@ -1890,7 +1907,7 @@
     </row>
     <row r="55" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="25" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B55" t="s">
         <v>27</v>
@@ -1906,7 +1923,7 @@
     </row>
     <row r="56" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="25" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B56" t="s">
         <v>56</v>
@@ -1922,14 +1939,14 @@
     </row>
     <row r="57" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="25" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B57" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C57" s="10"/>
       <c r="D57" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E57" s="10"/>
       <c r="F57" s="10" t="s">
@@ -1938,14 +1955,14 @@
     </row>
     <row r="58" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="25" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B58" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C58" s="10"/>
       <c r="D58" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E58" s="10"/>
       <c r="F58" s="10" t="s">
@@ -1954,14 +1971,14 @@
     </row>
     <row r="59" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="25" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B59" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C59" s="10"/>
       <c r="D59" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E59" s="10"/>
       <c r="F59" s="10" t="s">
@@ -1970,14 +1987,14 @@
     </row>
     <row r="60" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="25" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B60" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C60" s="10"/>
       <c r="D60" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E60" s="10"/>
       <c r="F60" s="10" t="s">
@@ -1986,7 +2003,7 @@
     </row>
     <row r="61" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B61" t="s">
         <v>29</v>
@@ -1995,14 +2012,16 @@
       <c r="D61" t="s">
         <v>11</v>
       </c>
-      <c r="E61" s="6"/>
+      <c r="E61" s="6" t="s">
+        <v>135</v>
+      </c>
       <c r="F61" s="10" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="25" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B62" t="s">
         <v>31</v>
@@ -2011,14 +2030,16 @@
       <c r="D62" t="s">
         <v>11</v>
       </c>
-      <c r="E62" s="6"/>
+      <c r="E62" s="6" t="s">
+        <v>135</v>
+      </c>
       <c r="F62" s="10" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" s="25" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B63" t="s">
         <v>32</v>
@@ -2027,14 +2048,16 @@
       <c r="D63" t="s">
         <v>11</v>
       </c>
-      <c r="E63" s="6"/>
+      <c r="E63" s="6" t="s">
+        <v>135</v>
+      </c>
       <c r="F63" s="10" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A64" s="25" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B64" t="s">
         <v>33</v>
@@ -2050,7 +2073,7 @@
     </row>
     <row r="65" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A65" s="25" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B65" t="s">
         <v>34</v>
@@ -2066,7 +2089,7 @@
     </row>
     <row r="66" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A66" s="25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B66" t="s">
         <v>35</v>
@@ -2082,7 +2105,7 @@
     </row>
     <row r="67" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A67" s="25" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B67" t="s">
         <v>36</v>
@@ -2098,7 +2121,7 @@
     </row>
     <row r="68" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A68" s="25" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B68" t="s">
         <v>39</v>
@@ -2114,7 +2137,7 @@
     </row>
     <row r="69" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A69" s="25" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B69" t="s">
         <v>40</v>
@@ -2130,7 +2153,7 @@
     </row>
     <row r="70" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A70" s="25" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B70" t="s">
         <v>41</v>
@@ -2145,9 +2168,22 @@
       </c>
     </row>
     <row r="71" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A71" s="25" t="s">
+        <v>133</v>
+      </c>
+      <c r="B71" t="s">
+        <v>134</v>
+      </c>
       <c r="C71" s="6"/>
-      <c r="E71" s="6"/>
-      <c r="F71" s="6"/>
+      <c r="D71" t="s">
+        <v>11</v>
+      </c>
+      <c r="E71" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="F71" s="6" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="72" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C72" s="6"/>

</xml_diff>

<commit_message>
updated test cases and test cases plan
</commit_message>
<xml_diff>
--- a/tests/TestCasesPlan.xlsx
+++ b/tests/TestCasesPlan.xlsx
@@ -378,12 +378,6 @@
     <t>projectDeleteAllRecords</t>
   </si>
   <si>
-    <t>projectDetailsAddUser</t>
-  </si>
-  <si>
-    <t>projectDetailsEdit</t>
-  </si>
-  <si>
     <t>projectDetailsDelete</t>
   </si>
   <si>
@@ -427,6 +421,12 @@
   </si>
   <si>
     <t>Pending</t>
+  </si>
+  <si>
+    <t>projectDetailAddUser</t>
+  </si>
+  <si>
+    <t>projectDetailEditUser</t>
   </si>
 </sst>
 </file>
@@ -452,6 +452,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -459,28 +460,33 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -488,11 +494,13 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -869,7 +877,7 @@
   <dimension ref="A1:AA1024"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="G61" sqref="G61"/>
+      <selection activeCell="E63" sqref="E63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -903,7 +911,7 @@
     </row>
     <row r="2" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="22" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>6</v>
@@ -921,7 +929,7 @@
     </row>
     <row r="3" spans="1:6" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A3" s="22" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>7</v>
@@ -972,7 +980,7 @@
         <v>68</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="14" t="s">
@@ -1298,7 +1306,7 @@
         <v>85</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C25" s="10"/>
       <c r="D25" s="15" t="s">
@@ -2003,7 +2011,7 @@
     </row>
     <row r="61" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="25" t="s">
-        <v>119</v>
+        <v>134</v>
       </c>
       <c r="B61" t="s">
         <v>29</v>
@@ -2021,7 +2029,7 @@
     </row>
     <row r="62" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="25" t="s">
-        <v>120</v>
+        <v>135</v>
       </c>
       <c r="B62" t="s">
         <v>31</v>
@@ -2039,7 +2047,7 @@
     </row>
     <row r="63" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" s="25" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B63" t="s">
         <v>32</v>
@@ -2049,7 +2057,7 @@
         <v>11</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>135</v>
+        <v>37</v>
       </c>
       <c r="F63" s="10" t="s">
         <v>38</v>
@@ -2057,7 +2065,7 @@
     </row>
     <row r="64" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A64" s="25" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B64" t="s">
         <v>33</v>
@@ -2073,7 +2081,7 @@
     </row>
     <row r="65" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A65" s="25" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B65" t="s">
         <v>34</v>
@@ -2089,7 +2097,7 @@
     </row>
     <row r="66" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A66" s="25" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B66" t="s">
         <v>35</v>
@@ -2105,7 +2113,7 @@
     </row>
     <row r="67" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A67" s="25" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B67" t="s">
         <v>36</v>
@@ -2121,7 +2129,7 @@
     </row>
     <row r="68" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A68" s="25" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B68" t="s">
         <v>39</v>
@@ -2137,7 +2145,7 @@
     </row>
     <row r="69" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A69" s="25" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B69" t="s">
         <v>40</v>
@@ -2153,7 +2161,7 @@
     </row>
     <row r="70" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A70" s="25" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B70" t="s">
         <v>41</v>
@@ -2169,17 +2177,17 @@
     </row>
     <row r="71" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A71" s="25" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B71" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C71" s="6"/>
       <c r="D71" t="s">
         <v>11</v>
       </c>
       <c r="E71" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F71" s="6" t="s">
         <v>38</v>

</xml_diff>

<commit_message>
uploaded all the complete test cases
</commit_message>
<xml_diff>
--- a/tests/TestCasesPlan.xlsx
+++ b/tests/TestCasesPlan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MYDOC\ILTWORKS\iltTests\tests\ExpoloaderNewTest\GitHub\ExpoloaderManagement\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MYDOC\ILTWORKS\iltTests\tests\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="136">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -424,6 +424,9 @@
   </si>
   <si>
     <t>projectDetailEditUser</t>
+  </si>
+  <si>
+    <t>Pending</t>
   </si>
 </sst>
 </file>
@@ -600,7 +603,175 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="28">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCC0000"/>
+          <bgColor rgb="FFCC0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF6AA84F"/>
+          <bgColor rgb="FF6AA84F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF9900"/>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCC0000"/>
+          <bgColor rgb="FFCC0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF6AA84F"/>
+          <bgColor rgb="FF6AA84F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF9900"/>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCC0000"/>
+          <bgColor rgb="FFCC0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF6AA84F"/>
+          <bgColor rgb="FF6AA84F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF9900"/>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCC0000"/>
+          <bgColor rgb="FFCC0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF6AA84F"/>
+          <bgColor rgb="FF6AA84F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF9900"/>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCC0000"/>
+          <bgColor rgb="FFCC0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF6AA84F"/>
+          <bgColor rgb="FF6AA84F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF9900"/>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCC0000"/>
+          <bgColor rgb="FFCC0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF6AA84F"/>
+          <bgColor rgb="FF6AA84F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF9900"/>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCC0000"/>
+          <bgColor rgb="FFCC0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF6AA84F"/>
+          <bgColor rgb="FF6AA84F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF9900"/>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -873,8 +1044,8 @@
   </sheetPr>
   <dimension ref="A1:AA1024"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="E71" sqref="E71"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -935,7 +1106,9 @@
       <c r="D3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="6"/>
+      <c r="E3" s="10" t="s">
+        <v>37</v>
+      </c>
       <c r="F3" s="10" t="s">
         <v>38</v>
       </c>
@@ -951,7 +1124,9 @@
       <c r="D4" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="6"/>
+      <c r="E4" s="10" t="s">
+        <v>37</v>
+      </c>
       <c r="F4" s="10" t="s">
         <v>38</v>
       </c>
@@ -967,7 +1142,9 @@
       <c r="D5" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="6"/>
+      <c r="E5" s="10" t="s">
+        <v>37</v>
+      </c>
       <c r="F5" s="10" t="s">
         <v>38</v>
       </c>
@@ -983,7 +1160,9 @@
       <c r="D6" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="6"/>
+      <c r="E6" s="10" t="s">
+        <v>37</v>
+      </c>
       <c r="F6" s="10" t="s">
         <v>38</v>
       </c>
@@ -999,7 +1178,9 @@
       <c r="D7" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="6"/>
+      <c r="E7" s="10" t="s">
+        <v>37</v>
+      </c>
       <c r="F7" s="10" t="s">
         <v>38</v>
       </c>
@@ -1087,7 +1268,9 @@
       <c r="D12" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="6"/>
+      <c r="E12" s="10" t="s">
+        <v>37</v>
+      </c>
       <c r="F12" s="10" t="s">
         <v>38</v>
       </c>
@@ -1103,7 +1286,9 @@
       <c r="D13" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="6"/>
+      <c r="E13" s="10" t="s">
+        <v>37</v>
+      </c>
       <c r="F13" s="10" t="s">
         <v>38</v>
       </c>
@@ -1119,7 +1304,9 @@
       <c r="D14" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="6"/>
+      <c r="E14" s="10" t="s">
+        <v>37</v>
+      </c>
       <c r="F14" s="10" t="s">
         <v>38</v>
       </c>
@@ -1135,7 +1322,9 @@
       <c r="D15" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="6"/>
+      <c r="E15" s="10" t="s">
+        <v>37</v>
+      </c>
       <c r="F15" s="10" t="s">
         <v>38</v>
       </c>
@@ -1151,7 +1340,9 @@
       <c r="D16" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="6"/>
+      <c r="E16" s="10" t="s">
+        <v>37</v>
+      </c>
       <c r="F16" s="10" t="s">
         <v>38</v>
       </c>
@@ -1167,7 +1358,9 @@
       <c r="D17" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="E17" s="6"/>
+      <c r="E17" s="10" t="s">
+        <v>37</v>
+      </c>
       <c r="F17" s="10" t="s">
         <v>38</v>
       </c>
@@ -1327,7 +1520,9 @@
       <c r="D26" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="E26" s="6"/>
+      <c r="E26" s="10" t="s">
+        <v>37</v>
+      </c>
       <c r="F26" s="10" t="s">
         <v>38</v>
       </c>
@@ -1343,7 +1538,9 @@
       <c r="D27" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="E27" s="6"/>
+      <c r="E27" s="10" t="s">
+        <v>37</v>
+      </c>
       <c r="F27" s="10" t="s">
         <v>38</v>
       </c>
@@ -1380,7 +1577,9 @@
       <c r="D28" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="E28" s="10"/>
+      <c r="E28" s="10" t="s">
+        <v>37</v>
+      </c>
       <c r="F28" s="10" t="s">
         <v>38</v>
       </c>
@@ -1456,7 +1655,9 @@
       <c r="D30" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="E30" s="6"/>
+      <c r="E30" s="10" t="s">
+        <v>37</v>
+      </c>
       <c r="F30" s="10" t="s">
         <v>38</v>
       </c>
@@ -1493,7 +1694,9 @@
       <c r="D31" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="E31" s="6"/>
+      <c r="E31" s="10" t="s">
+        <v>37</v>
+      </c>
       <c r="F31" s="10" t="s">
         <v>38</v>
       </c>
@@ -1530,7 +1733,9 @@
       <c r="D32" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="E32" s="6"/>
+      <c r="E32" s="10" t="s">
+        <v>37</v>
+      </c>
       <c r="F32" s="10" t="s">
         <v>38</v>
       </c>
@@ -1585,7 +1790,9 @@
       <c r="D34" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="E34" s="6"/>
+      <c r="E34" s="6" t="s">
+        <v>135</v>
+      </c>
       <c r="F34" s="10" t="s">
         <v>38</v>
       </c>
@@ -1601,7 +1808,9 @@
       <c r="D35" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="E35" s="6"/>
+      <c r="E35" s="10" t="s">
+        <v>135</v>
+      </c>
       <c r="F35" s="10" t="s">
         <v>38</v>
       </c>
@@ -1617,7 +1826,9 @@
       <c r="D36" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="E36" s="6"/>
+      <c r="E36" s="10" t="s">
+        <v>135</v>
+      </c>
       <c r="F36" s="10" t="s">
         <v>38</v>
       </c>
@@ -1633,7 +1844,9 @@
       <c r="D37" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="E37" s="6"/>
+      <c r="E37" s="10" t="s">
+        <v>135</v>
+      </c>
       <c r="F37" s="10" t="s">
         <v>38</v>
       </c>
@@ -1649,7 +1862,9 @@
       <c r="D38" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="E38" s="6"/>
+      <c r="E38" s="10" t="s">
+        <v>135</v>
+      </c>
       <c r="F38" s="10" t="s">
         <v>38</v>
       </c>
@@ -1665,7 +1880,9 @@
       <c r="D39" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="E39" s="6"/>
+      <c r="E39" s="10" t="s">
+        <v>135</v>
+      </c>
       <c r="F39" s="10" t="s">
         <v>38</v>
       </c>
@@ -1681,7 +1898,9 @@
       <c r="D40" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="E40" s="6"/>
+      <c r="E40" s="10" t="s">
+        <v>135</v>
+      </c>
       <c r="F40" s="10" t="s">
         <v>38</v>
       </c>
@@ -1697,7 +1916,9 @@
       <c r="D41" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="E41" s="6"/>
+      <c r="E41" s="10" t="s">
+        <v>135</v>
+      </c>
       <c r="F41" s="10" t="s">
         <v>38</v>
       </c>
@@ -1713,7 +1934,9 @@
       <c r="D42" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="E42" s="6"/>
+      <c r="E42" s="10" t="s">
+        <v>135</v>
+      </c>
       <c r="F42" s="10" t="s">
         <v>38</v>
       </c>
@@ -1729,7 +1952,9 @@
       <c r="D43" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="E43" s="6"/>
+      <c r="E43" s="10" t="s">
+        <v>135</v>
+      </c>
       <c r="F43" s="10" t="s">
         <v>38</v>
       </c>
@@ -1745,7 +1970,9 @@
       <c r="D44" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="E44" s="6"/>
+      <c r="E44" s="10" t="s">
+        <v>135</v>
+      </c>
       <c r="F44" s="10" t="s">
         <v>38</v>
       </c>
@@ -1761,7 +1988,9 @@
       <c r="D45" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="E45" s="6"/>
+      <c r="E45" s="10" t="s">
+        <v>135</v>
+      </c>
       <c r="F45" s="10" t="s">
         <v>38</v>
       </c>
@@ -1777,7 +2006,9 @@
       <c r="D46" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="E46" s="6"/>
+      <c r="E46" s="10" t="s">
+        <v>135</v>
+      </c>
       <c r="F46" s="10" t="s">
         <v>38</v>
       </c>
@@ -1793,7 +2024,9 @@
       <c r="D47" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="E47" s="6"/>
+      <c r="E47" s="10" t="s">
+        <v>135</v>
+      </c>
       <c r="F47" s="10" t="s">
         <v>38</v>
       </c>
@@ -1809,7 +2042,9 @@
       <c r="D48" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="E48" s="6"/>
+      <c r="E48" s="10" t="s">
+        <v>135</v>
+      </c>
       <c r="F48" s="10" t="s">
         <v>38</v>
       </c>
@@ -1825,7 +2060,9 @@
       <c r="D49" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="E49" s="6"/>
+      <c r="E49" s="10" t="s">
+        <v>135</v>
+      </c>
       <c r="F49" s="10" t="s">
         <v>38</v>
       </c>
@@ -1841,7 +2078,9 @@
       <c r="D50" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="E50" s="6"/>
+      <c r="E50" s="10" t="s">
+        <v>135</v>
+      </c>
       <c r="F50" s="10" t="s">
         <v>38</v>
       </c>
@@ -1857,7 +2096,9 @@
       <c r="D51" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="E51" s="6"/>
+      <c r="E51" s="10" t="s">
+        <v>135</v>
+      </c>
       <c r="F51" s="10" t="s">
         <v>38</v>
       </c>
@@ -1873,7 +2114,9 @@
       <c r="D52" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="E52" s="6"/>
+      <c r="E52" s="10" t="s">
+        <v>135</v>
+      </c>
       <c r="F52" s="10" t="s">
         <v>38</v>
       </c>
@@ -1889,7 +2132,9 @@
       <c r="D53" t="s">
         <v>53</v>
       </c>
-      <c r="E53" s="6"/>
+      <c r="E53" s="10" t="s">
+        <v>135</v>
+      </c>
       <c r="F53" s="10" t="s">
         <v>38</v>
       </c>
@@ -1905,7 +2150,9 @@
       <c r="D54" t="s">
         <v>53</v>
       </c>
-      <c r="E54" s="6"/>
+      <c r="E54" s="10" t="s">
+        <v>135</v>
+      </c>
       <c r="F54" s="10" t="s">
         <v>38</v>
       </c>
@@ -1921,7 +2168,9 @@
       <c r="D55" t="s">
         <v>53</v>
       </c>
-      <c r="E55" s="6"/>
+      <c r="E55" s="10" t="s">
+        <v>135</v>
+      </c>
       <c r="F55" s="10" t="s">
         <v>38</v>
       </c>
@@ -1937,7 +2186,9 @@
       <c r="D56" t="s">
         <v>8</v>
       </c>
-      <c r="E56" s="6"/>
+      <c r="E56" s="10" t="s">
+        <v>37</v>
+      </c>
       <c r="F56" s="10" t="s">
         <v>38</v>
       </c>
@@ -1953,7 +2204,9 @@
       <c r="D57" t="s">
         <v>60</v>
       </c>
-      <c r="E57" s="10"/>
+      <c r="E57" s="10" t="s">
+        <v>37</v>
+      </c>
       <c r="F57" s="10" t="s">
         <v>38</v>
       </c>
@@ -1969,7 +2222,9 @@
       <c r="D58" t="s">
         <v>60</v>
       </c>
-      <c r="E58" s="10"/>
+      <c r="E58" s="10" t="s">
+        <v>37</v>
+      </c>
       <c r="F58" s="10" t="s">
         <v>38</v>
       </c>
@@ -1985,7 +2240,9 @@
       <c r="D59" t="s">
         <v>60</v>
       </c>
-      <c r="E59" s="10"/>
+      <c r="E59" s="10" t="s">
+        <v>37</v>
+      </c>
       <c r="F59" s="10" t="s">
         <v>38</v>
       </c>
@@ -2001,7 +2258,9 @@
       <c r="D60" t="s">
         <v>60</v>
       </c>
-      <c r="E60" s="10"/>
+      <c r="E60" s="10" t="s">
+        <v>37</v>
+      </c>
       <c r="F60" s="10" t="s">
         <v>38</v>
       </c>
@@ -2071,7 +2330,9 @@
       <c r="D64" t="s">
         <v>23</v>
       </c>
-      <c r="E64" s="6"/>
+      <c r="E64" s="10" t="s">
+        <v>37</v>
+      </c>
       <c r="F64" s="10" t="s">
         <v>38</v>
       </c>
@@ -2087,7 +2348,9 @@
       <c r="D65" t="s">
         <v>23</v>
       </c>
-      <c r="E65" s="6"/>
+      <c r="E65" s="10" t="s">
+        <v>37</v>
+      </c>
       <c r="F65" s="10" t="s">
         <v>38</v>
       </c>
@@ -2103,7 +2366,9 @@
       <c r="D66" t="s">
         <v>30</v>
       </c>
-      <c r="E66" s="6"/>
+      <c r="E66" s="10" t="s">
+        <v>37</v>
+      </c>
       <c r="F66" s="10" t="s">
         <v>38</v>
       </c>
@@ -2119,7 +2384,9 @@
       <c r="D67" t="s">
         <v>30</v>
       </c>
-      <c r="E67" s="6"/>
+      <c r="E67" s="10" t="s">
+        <v>37</v>
+      </c>
       <c r="F67" s="10" t="s">
         <v>38</v>
       </c>
@@ -2135,7 +2402,9 @@
       <c r="D68" t="s">
         <v>9</v>
       </c>
-      <c r="E68" s="6"/>
+      <c r="E68" s="10" t="s">
+        <v>37</v>
+      </c>
       <c r="F68" s="10" t="s">
         <v>38</v>
       </c>
@@ -2151,7 +2420,9 @@
       <c r="D69" t="s">
         <v>28</v>
       </c>
-      <c r="E69" s="6"/>
+      <c r="E69" s="6" t="s">
+        <v>135</v>
+      </c>
       <c r="F69" s="10" t="s">
         <v>38</v>
       </c>
@@ -2167,7 +2438,9 @@
       <c r="D70" t="s">
         <v>28</v>
       </c>
-      <c r="E70" s="6"/>
+      <c r="E70" s="6" t="s">
+        <v>135</v>
+      </c>
       <c r="F70" s="10" t="s">
         <v>38</v>
       </c>
@@ -6940,37 +7213,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F2:F1024">
-    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="5" operator="equal">
       <formula>"Developed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:F56 E61:F1024 F57:F60">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+  <conditionalFormatting sqref="E2:F1024">
+    <cfRule type="cellIs" dxfId="26" priority="6" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E56 E61:E1024">
-    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
+  <conditionalFormatting sqref="E2:E1024">
+    <cfRule type="cellIs" dxfId="25" priority="7" operator="equal">
       <formula>"Tested"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E56 E61:E1024">
-    <cfRule type="cellIs" dxfId="3" priority="9" operator="equal">
-      <formula>"Issue"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E57:E60">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
-      <formula>"Pending"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E57:E60">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
-      <formula>"Tested"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E57:E60">
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+  <conditionalFormatting sqref="E2:E1024">
+    <cfRule type="cellIs" dxfId="24" priority="9" operator="equal">
       <formula>"Issue"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>